<commit_message>
Site updated: 2023-07-05 10:44:32
</commit_message>
<xml_diff>
--- a/resources/gohsc-policy-indicator-checklist.xlsx
+++ b/resources/gohsc-policy-indicator-checklist.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="23" documentId="8_{6584D590-C07C-4F62-BFAE-96514BB22693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E04B985-D556-4F83-8B31-521652B07492}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CBD1D931-24DA-4E3E-B988-2C7CFFF38AFE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{CBD1D931-24DA-4E3E-B988-2C7CFFF38AFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -2832,13 +2832,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2846,14 +2839,21 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2865,19 +2865,92 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2885,19 +2958,7 @@
     <xf numFmtId="0" fontId="21" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2912,24 +2973,21 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2939,68 +2997,10 @@
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3515,7 +3515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B58290-3ADE-464D-B178-F7852B2419A2}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -3537,35 +3537,35 @@
       <c r="C2" s="94"/>
     </row>
     <row r="3" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="200" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="203"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="204"/>
-      <c r="B4" s="204"/>
-      <c r="C4" s="204"/>
+      <c r="A4" s="201"/>
+      <c r="B4" s="201"/>
+      <c r="C4" s="201"/>
     </row>
     <row r="5" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="205" t="s">
+      <c r="A5" s="202" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="205"/>
-      <c r="C5" s="205"/>
+      <c r="B5" s="202"/>
+      <c r="C5" s="202"/>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="204"/>
-      <c r="B6" s="204"/>
-      <c r="C6" s="204"/>
+      <c r="A6" s="201"/>
+      <c r="B6" s="201"/>
+      <c r="C6" s="201"/>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="202" t="s">
+      <c r="A7" s="203" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="202"/>
-      <c r="C7" s="202"/>
+      <c r="B7" s="203"/>
+      <c r="C7" s="203"/>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="106" t="s">
@@ -3636,11 +3636,11 @@
       <c r="C15" s="107"/>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="202" t="s">
+      <c r="A16" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="202"/>
-      <c r="C16" s="202"/>
+      <c r="B16" s="203"/>
+      <c r="C16" s="203"/>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="106" t="s">
@@ -3727,10 +3727,10 @@
       <c r="A26" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="200" t="s">
+      <c r="B26" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="200"/>
+      <c r="C26" s="204"/>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="53"/>
@@ -3765,11 +3765,11 @@
       <c r="C30" s="108"/>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="201" t="s">
+      <c r="A31" s="205" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="201"/>
-      <c r="C31" s="201"/>
+      <c r="B31" s="205"/>
+      <c r="C31" s="205"/>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="106" t="s">
@@ -3795,11 +3795,11 @@
       <c r="C34" s="108"/>
     </row>
     <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="201" t="s">
+      <c r="A35" s="205" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="201"/>
-      <c r="C35" s="201"/>
+      <c r="B35" s="205"/>
+      <c r="C35" s="205"/>
     </row>
     <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="106" t="s">
@@ -3821,16 +3821,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B26:C26"/>
@@ -3841,6 +3831,16 @@
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="B24:C24"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C25" r:id="rId1" display="○ To view more details on how to insert a new row, click here" xr:uid="{45345299-ED7E-47D8-AEAE-79F712512FF9}"/>
@@ -3881,11 +3881,11 @@
       <c r="C2" s="94"/>
     </row>
     <row r="3" spans="1:3" s="181" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="203" t="s">
+      <c r="A3" s="200" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="203"/>
-      <c r="C3" s="203"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="209"/>
@@ -3942,10 +3942,10 @@
       <c r="C11" s="110"/>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="206" t="s">
+      <c r="A12" s="207" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="207"/>
+      <c r="B12" s="208"/>
       <c r="C12" s="172"/>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3998,80 +3998,80 @@
       <c r="C19" s="171"/>
     </row>
     <row r="20" spans="1:3" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="206" t="s">
+      <c r="A20" s="207" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="206"/>
+      <c r="B20" s="207"/>
       <c r="C20" s="173"/>
     </row>
     <row r="21" spans="1:3" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="206" t="s">
+      <c r="A21" s="207" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="206"/>
+      <c r="B21" s="207"/>
       <c r="C21" s="111"/>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="208" t="s">
+      <c r="A22" s="206" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="208"/>
+      <c r="B22" s="206"/>
       <c r="C22" s="174"/>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="208" t="s">
+      <c r="A23" s="206" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="208"/>
+      <c r="B23" s="206"/>
       <c r="C23" s="175"/>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="208" t="s">
+      <c r="A24" s="206" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="208"/>
+      <c r="B24" s="206"/>
       <c r="C24" s="175"/>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="208" t="s">
+      <c r="A25" s="206" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="208"/>
+      <c r="B25" s="206"/>
       <c r="C25" s="175"/>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="208" t="s">
+      <c r="A26" s="206" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="208"/>
+      <c r="B26" s="206"/>
       <c r="C26" s="175"/>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="208" t="s">
+      <c r="A27" s="206" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="208"/>
+      <c r="B27" s="206"/>
       <c r="C27" s="176"/>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="208" t="s">
+      <c r="A28" s="206" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="208"/>
+      <c r="B28" s="206"/>
       <c r="C28" s="176"/>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="208" t="s">
+      <c r="A29" s="206" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="208"/>
+      <c r="B29" s="206"/>
       <c r="C29" s="176"/>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="208" t="s">
+      <c r="A30" s="206" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="208"/>
+      <c r="B30" s="206"/>
       <c r="C30" s="175"/>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4084,14 +4084,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A21:B21"/>
@@ -4102,6 +4094,14 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="No/Yes" prompt="Please select response from drop down" sqref="C22:C30" xr:uid="{7200986C-DC30-4512-8BE1-5C41BF347B27}">
@@ -4121,11 +4121,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFECF44-670A-42DD-8E77-1B9AE269ADAB}">
   <dimension ref="A1:N288"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4143,38 +4143,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="182" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="214" t="s">
+      <c r="A1" s="255" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="214"/>
-      <c r="C1" s="215"/>
-      <c r="D1" s="218" t="s">
+      <c r="B1" s="255"/>
+      <c r="C1" s="256"/>
+      <c r="D1" s="241" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="218" t="s">
+      <c r="E1" s="241" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="218" t="s">
+      <c r="F1" s="241" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="218" t="s">
+      <c r="G1" s="241" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="216" t="s">
+      <c r="H1" s="249" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="218" t="s">
+      <c r="I1" s="241" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="232" t="s">
+      <c r="J1" s="248" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="216"/>
-      <c r="L1" s="235" t="s">
+      <c r="K1" s="249"/>
+      <c r="L1" s="253" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="216"/>
-      <c r="N1" s="218" t="s">
+      <c r="M1" s="249"/>
+      <c r="N1" s="241" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4184,17 +4184,17 @@
       </c>
       <c r="B2" s="190"/>
       <c r="C2" s="191"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
-      <c r="H2" s="217"/>
-      <c r="I2" s="219"/>
-      <c r="J2" s="233"/>
-      <c r="K2" s="217"/>
-      <c r="L2" s="236"/>
-      <c r="M2" s="217"/>
-      <c r="N2" s="219"/>
+      <c r="D2" s="242"/>
+      <c r="E2" s="242"/>
+      <c r="F2" s="242"/>
+      <c r="G2" s="242"/>
+      <c r="H2" s="251"/>
+      <c r="I2" s="242"/>
+      <c r="J2" s="250"/>
+      <c r="K2" s="251"/>
+      <c r="L2" s="254"/>
+      <c r="M2" s="251"/>
+      <c r="N2" s="242"/>
     </row>
     <row r="3" spans="1:14" s="182" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="145" t="s">
@@ -4206,7 +4206,7 @@
       <c r="C3" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="220"/>
+      <c r="D3" s="257"/>
       <c r="E3" s="178" t="s">
         <v>74</v>
       </c>
@@ -4309,11 +4309,11 @@
       <c r="N5" s="102"/>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="234" t="s">
+      <c r="A6" s="252" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="234"/>
-      <c r="C6" s="234"/>
+      <c r="B6" s="252"/>
+      <c r="C6" s="252"/>
       <c r="D6" s="67"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -4327,11 +4327,11 @@
       <c r="N6" s="36"/>
     </row>
     <row r="7" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="230" t="s">
+      <c r="A7" s="223" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="230"/>
-      <c r="C7" s="231"/>
+      <c r="B7" s="223"/>
+      <c r="C7" s="247"/>
       <c r="D7" s="68"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -4345,33 +4345,33 @@
       <c r="N7" s="37"/>
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="228" t="s">
+      <c r="A8" s="217" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="242" t="s">
+      <c r="B8" s="233" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="252"/>
+      <c r="C8" s="234"/>
       <c r="D8" s="50"/>
       <c r="E8" s="65"/>
-      <c r="F8" s="244" t="s">
+      <c r="F8" s="225" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="245"/>
-      <c r="H8" s="245"/>
-      <c r="I8" s="245"/>
-      <c r="J8" s="245"/>
-      <c r="K8" s="245"/>
-      <c r="L8" s="245"/>
-      <c r="M8" s="246"/>
+      <c r="G8" s="226"/>
+      <c r="H8" s="226"/>
+      <c r="I8" s="226"/>
+      <c r="J8" s="226"/>
+      <c r="K8" s="226"/>
+      <c r="L8" s="226"/>
+      <c r="M8" s="227"/>
       <c r="N8" s="38"/>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="228"/>
-      <c r="B9" s="247" t="s">
+      <c r="A9" s="217"/>
+      <c r="B9" s="228" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="248"/>
+      <c r="C9" s="229"/>
       <c r="D9" s="23"/>
       <c r="E9" s="65"/>
       <c r="F9" s="56"/>
@@ -4385,11 +4385,11 @@
       <c r="N9" s="39"/>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="228"/>
-      <c r="B10" s="247" t="s">
+      <c r="A10" s="217"/>
+      <c r="B10" s="228" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="248"/>
+      <c r="C10" s="229"/>
       <c r="D10" s="23"/>
       <c r="E10" s="65"/>
       <c r="F10" s="46"/>
@@ -4403,11 +4403,11 @@
       <c r="N10" s="39"/>
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="228"/>
-      <c r="B11" s="247" t="s">
+      <c r="A11" s="217"/>
+      <c r="B11" s="228" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="248"/>
+      <c r="C11" s="229"/>
       <c r="D11" s="23"/>
       <c r="E11" s="65"/>
       <c r="F11" s="46"/>
@@ -4421,8 +4421,8 @@
       <c r="N11" s="39"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="228"/>
-      <c r="B12" s="249" t="s">
+      <c r="A12" s="217"/>
+      <c r="B12" s="230" t="s">
         <v>101</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -4441,8 +4441,8 @@
       <c r="N12" s="9"/>
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="228"/>
-      <c r="B13" s="250"/>
+      <c r="A13" s="217"/>
+      <c r="B13" s="231"/>
       <c r="C13" s="150" t="s">
         <v>103</v>
       </c>
@@ -4459,8 +4459,8 @@
       <c r="N13" s="30"/>
     </row>
     <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="228"/>
-      <c r="B14" s="250"/>
+      <c r="A14" s="217"/>
+      <c r="B14" s="231"/>
       <c r="C14" s="151" t="s">
         <v>104</v>
       </c>
@@ -4477,8 +4477,8 @@
       <c r="N14" s="25"/>
     </row>
     <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="228"/>
-      <c r="B15" s="250"/>
+      <c r="A15" s="217"/>
+      <c r="B15" s="231"/>
       <c r="C15" s="151" t="s">
         <v>105</v>
       </c>
@@ -4495,8 +4495,8 @@
       <c r="N15" s="25"/>
     </row>
     <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="229"/>
-      <c r="B16" s="251"/>
+      <c r="A16" s="218"/>
+      <c r="B16" s="232"/>
       <c r="C16" s="152" t="s">
         <v>106</v>
       </c>
@@ -4513,11 +4513,11 @@
       <c r="N16" s="26"/>
     </row>
     <row r="17" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="230" t="s">
+      <c r="A17" s="223" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="230"/>
-      <c r="C17" s="230"/>
+      <c r="B17" s="223"/>
+      <c r="C17" s="223"/>
       <c r="D17" s="70"/>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
@@ -4531,10 +4531,10 @@
       <c r="N17" s="42"/>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="228" t="s">
+      <c r="A18" s="217" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="221" t="s">
+      <c r="B18" s="213" t="s">
         <v>109</v>
       </c>
       <c r="C18" s="43" t="s">
@@ -4553,8 +4553,8 @@
       <c r="N18" s="44"/>
     </row>
     <row r="19" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="228"/>
-      <c r="B19" s="221"/>
+      <c r="A19" s="217"/>
+      <c r="B19" s="213"/>
       <c r="C19" s="153" t="s">
         <v>110</v>
       </c>
@@ -4571,7 +4571,7 @@
       <c r="N19" s="24"/>
     </row>
     <row r="20" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="228"/>
+      <c r="A20" s="217"/>
       <c r="B20" s="33" t="s">
         <v>111</v>
       </c>
@@ -4591,8 +4591,8 @@
       <c r="N20" s="25"/>
     </row>
     <row r="21" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="228"/>
-      <c r="B21" s="212" t="s">
+      <c r="A21" s="217"/>
+      <c r="B21" s="221" t="s">
         <v>113</v>
       </c>
       <c r="C21" s="154" t="s">
@@ -4611,8 +4611,8 @@
       <c r="N21" s="25"/>
     </row>
     <row r="22" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="228"/>
-      <c r="B22" s="212"/>
+      <c r="A22" s="217"/>
+      <c r="B22" s="221"/>
       <c r="C22" s="154" t="s">
         <v>115</v>
       </c>
@@ -4629,8 +4629,8 @@
       <c r="N22" s="25"/>
     </row>
     <row r="23" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="228"/>
-      <c r="B23" s="212"/>
+      <c r="A23" s="217"/>
+      <c r="B23" s="221"/>
       <c r="C23" s="154" t="s">
         <v>116</v>
       </c>
@@ -4647,8 +4647,8 @@
       <c r="N23" s="25"/>
     </row>
     <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="228"/>
-      <c r="B24" s="212" t="s">
+      <c r="A24" s="217"/>
+      <c r="B24" s="221" t="s">
         <v>117</v>
       </c>
       <c r="C24" s="154" t="s">
@@ -4667,8 +4667,8 @@
       <c r="N24" s="25"/>
     </row>
     <row r="25" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="228"/>
-      <c r="B25" s="212"/>
+      <c r="A25" s="217"/>
+      <c r="B25" s="221"/>
       <c r="C25" s="154" t="s">
         <v>119</v>
       </c>
@@ -4685,8 +4685,8 @@
       <c r="N25" s="25"/>
     </row>
     <row r="26" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="228"/>
-      <c r="B26" s="212"/>
+      <c r="A26" s="217"/>
+      <c r="B26" s="221"/>
       <c r="C26" s="154" t="s">
         <v>106</v>
       </c>
@@ -4703,8 +4703,8 @@
       <c r="N26" s="25"/>
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="228"/>
-      <c r="B27" s="212"/>
+      <c r="A27" s="217"/>
+      <c r="B27" s="221"/>
       <c r="C27" s="13" t="s">
         <v>85</v>
       </c>
@@ -4721,8 +4721,8 @@
       <c r="N27" s="8"/>
     </row>
     <row r="28" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="228"/>
-      <c r="B28" s="212"/>
+      <c r="A28" s="217"/>
+      <c r="B28" s="221"/>
       <c r="C28" s="153" t="s">
         <v>120</v>
       </c>
@@ -4739,8 +4739,8 @@
       <c r="N28" s="25"/>
     </row>
     <row r="29" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="228"/>
-      <c r="B29" s="212"/>
+      <c r="A29" s="217"/>
+      <c r="B29" s="221"/>
       <c r="C29" s="154" t="s">
         <v>121</v>
       </c>
@@ -4757,8 +4757,8 @@
       <c r="N29" s="25"/>
     </row>
     <row r="30" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="228"/>
-      <c r="B30" s="212"/>
+      <c r="A30" s="217"/>
+      <c r="B30" s="221"/>
       <c r="C30" s="154" t="s">
         <v>122</v>
       </c>
@@ -4775,8 +4775,8 @@
       <c r="N30" s="25"/>
     </row>
     <row r="31" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="228"/>
-      <c r="B31" s="213"/>
+      <c r="A31" s="217"/>
+      <c r="B31" s="236"/>
       <c r="C31" s="155" t="s">
         <v>106</v>
       </c>
@@ -4793,8 +4793,8 @@
       <c r="N31" s="26"/>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="228"/>
-      <c r="B32" s="223" t="s">
+      <c r="A32" s="217"/>
+      <c r="B32" s="212" t="s">
         <v>123</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -4813,8 +4813,8 @@
       <c r="N32" s="8"/>
     </row>
     <row r="33" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="228"/>
-      <c r="B33" s="221"/>
+      <c r="A33" s="217"/>
+      <c r="B33" s="213"/>
       <c r="C33" s="153" t="s">
         <v>124</v>
       </c>
@@ -4831,8 +4831,8 @@
       <c r="N33" s="24"/>
     </row>
     <row r="34" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="228"/>
-      <c r="B34" s="221"/>
+      <c r="A34" s="217"/>
+      <c r="B34" s="213"/>
       <c r="C34" s="154" t="s">
         <v>125</v>
       </c>
@@ -4849,8 +4849,8 @@
       <c r="N34" s="25"/>
     </row>
     <row r="35" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="228"/>
-      <c r="B35" s="221"/>
+      <c r="A35" s="217"/>
+      <c r="B35" s="213"/>
       <c r="C35" s="154" t="s">
         <v>126</v>
       </c>
@@ -4867,8 +4867,8 @@
       <c r="N35" s="25"/>
     </row>
     <row r="36" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="228"/>
-      <c r="B36" s="221"/>
+      <c r="A36" s="217"/>
+      <c r="B36" s="213"/>
       <c r="C36" s="154" t="s">
         <v>127</v>
       </c>
@@ -4885,8 +4885,8 @@
       <c r="N36" s="25"/>
     </row>
     <row r="37" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="228"/>
-      <c r="B37" s="221"/>
+      <c r="A37" s="217"/>
+      <c r="B37" s="213"/>
       <c r="C37" s="154" t="s">
         <v>106</v>
       </c>
@@ -4903,8 +4903,8 @@
       <c r="N37" s="25"/>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="228"/>
-      <c r="B38" s="221"/>
+      <c r="A38" s="217"/>
+      <c r="B38" s="213"/>
       <c r="C38" s="13" t="s">
         <v>85</v>
       </c>
@@ -4921,8 +4921,8 @@
       <c r="N38" s="8"/>
     </row>
     <row r="39" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="228"/>
-      <c r="B39" s="221"/>
+      <c r="A39" s="217"/>
+      <c r="B39" s="213"/>
       <c r="C39" s="154" t="s">
         <v>128</v>
       </c>
@@ -4939,8 +4939,8 @@
       <c r="N39" s="25"/>
     </row>
     <row r="40" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="229"/>
-      <c r="B40" s="224"/>
+      <c r="A40" s="218"/>
+      <c r="B40" s="214"/>
       <c r="C40" s="155" t="s">
         <v>106</v>
       </c>
@@ -4957,11 +4957,11 @@
       <c r="N40" s="26"/>
     </row>
     <row r="41" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="230" t="s">
+      <c r="A41" s="223" t="s">
         <v>129</v>
       </c>
-      <c r="B41" s="230"/>
-      <c r="C41" s="230"/>
+      <c r="B41" s="223"/>
+      <c r="C41" s="223"/>
       <c r="D41" s="70"/>
       <c r="E41" s="42"/>
       <c r="F41" s="42"/>
@@ -4975,10 +4975,10 @@
       <c r="N41" s="42"/>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="228" t="s">
+      <c r="A42" s="217" t="s">
         <v>130</v>
       </c>
-      <c r="B42" s="221" t="s">
+      <c r="B42" s="213" t="s">
         <v>131</v>
       </c>
       <c r="C42" s="43" t="s">
@@ -4997,8 +4997,8 @@
       <c r="N42" s="44"/>
     </row>
     <row r="43" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="228"/>
-      <c r="B43" s="221"/>
+      <c r="A43" s="217"/>
+      <c r="B43" s="213"/>
       <c r="C43" s="153" t="s">
         <v>132</v>
       </c>
@@ -5015,8 +5015,8 @@
       <c r="N43" s="24"/>
     </row>
     <row r="44" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="228"/>
-      <c r="B44" s="221"/>
+      <c r="A44" s="217"/>
+      <c r="B44" s="213"/>
       <c r="C44" s="154" t="s">
         <v>133</v>
       </c>
@@ -5033,8 +5033,8 @@
       <c r="N44" s="25"/>
     </row>
     <row r="45" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="228"/>
-      <c r="B45" s="221"/>
+      <c r="A45" s="217"/>
+      <c r="B45" s="213"/>
       <c r="C45" s="154" t="s">
         <v>106</v>
       </c>
@@ -5051,8 +5051,8 @@
       <c r="N45" s="25"/>
     </row>
     <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="228"/>
-      <c r="B46" s="221"/>
+      <c r="A46" s="217"/>
+      <c r="B46" s="213"/>
       <c r="C46" s="13" t="s">
         <v>85</v>
       </c>
@@ -5069,8 +5069,8 @@
       <c r="N46" s="8"/>
     </row>
     <row r="47" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="228"/>
-      <c r="B47" s="221"/>
+      <c r="A47" s="217"/>
+      <c r="B47" s="213"/>
       <c r="C47" s="153" t="s">
         <v>134</v>
       </c>
@@ -5087,8 +5087,8 @@
       <c r="N47" s="25"/>
     </row>
     <row r="48" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="228"/>
-      <c r="B48" s="221"/>
+      <c r="A48" s="217"/>
+      <c r="B48" s="213"/>
       <c r="C48" s="154" t="s">
         <v>135</v>
       </c>
@@ -5105,8 +5105,8 @@
       <c r="N48" s="25"/>
     </row>
     <row r="49" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="229"/>
-      <c r="B49" s="221"/>
+      <c r="A49" s="218"/>
+      <c r="B49" s="213"/>
       <c r="C49" s="156" t="s">
         <v>106</v>
       </c>
@@ -5123,11 +5123,11 @@
       <c r="N49" s="28"/>
     </row>
     <row r="50" spans="1:14" s="185" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="230" t="s">
+      <c r="A50" s="223" t="s">
         <v>136</v>
       </c>
-      <c r="B50" s="230"/>
-      <c r="C50" s="231"/>
+      <c r="B50" s="223"/>
+      <c r="C50" s="247"/>
       <c r="D50" s="70"/>
       <c r="E50" s="42"/>
       <c r="F50" s="42"/>
@@ -5141,10 +5141,10 @@
       <c r="N50" s="45"/>
     </row>
     <row r="51" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="228" t="s">
+      <c r="A51" s="217" t="s">
         <v>137</v>
       </c>
-      <c r="B51" s="221" t="s">
+      <c r="B51" s="213" t="s">
         <v>138</v>
       </c>
       <c r="C51" s="43" t="s">
@@ -5163,8 +5163,8 @@
       <c r="N51" s="44"/>
     </row>
     <row r="52" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="228"/>
-      <c r="B52" s="221"/>
+      <c r="A52" s="217"/>
+      <c r="B52" s="213"/>
       <c r="C52" s="153" t="s">
         <v>139</v>
       </c>
@@ -5181,25 +5181,25 @@
       <c r="N52" s="24"/>
     </row>
     <row r="53" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="228"/>
-      <c r="B53" s="221"/>
+      <c r="A53" s="217"/>
+      <c r="B53" s="213"/>
       <c r="C53" s="154" t="s">
         <v>140</v>
       </c>
-      <c r="D53" s="225"/>
-      <c r="E53" s="226"/>
-      <c r="F53" s="226"/>
-      <c r="G53" s="226"/>
-      <c r="H53" s="226"/>
-      <c r="I53" s="226"/>
-      <c r="J53" s="226"/>
-      <c r="K53" s="226"/>
-      <c r="L53" s="226"/>
-      <c r="M53" s="226"/>
-      <c r="N53" s="227"/>
+      <c r="D53" s="244"/>
+      <c r="E53" s="245"/>
+      <c r="F53" s="245"/>
+      <c r="G53" s="245"/>
+      <c r="H53" s="245"/>
+      <c r="I53" s="245"/>
+      <c r="J53" s="245"/>
+      <c r="K53" s="245"/>
+      <c r="L53" s="245"/>
+      <c r="M53" s="245"/>
+      <c r="N53" s="246"/>
     </row>
     <row r="54" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="228"/>
+      <c r="A54" s="217"/>
       <c r="B54" s="33" t="s">
         <v>141</v>
       </c>
@@ -5219,8 +5219,8 @@
       <c r="N54" s="25"/>
     </row>
     <row r="55" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="228"/>
-      <c r="B55" s="254" t="s">
+      <c r="A55" s="217"/>
+      <c r="B55" s="216" t="s">
         <v>143</v>
       </c>
       <c r="C55" s="157" t="s">
@@ -5239,8 +5239,8 @@
       <c r="N55" s="25"/>
     </row>
     <row r="56" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="228"/>
-      <c r="B56" s="254"/>
+      <c r="A56" s="217"/>
+      <c r="B56" s="216"/>
       <c r="C56" s="157" t="s">
         <v>145</v>
       </c>
@@ -5257,8 +5257,8 @@
       <c r="N56" s="25"/>
     </row>
     <row r="57" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="228"/>
-      <c r="B57" s="254"/>
+      <c r="A57" s="217"/>
+      <c r="B57" s="216"/>
       <c r="C57" s="157" t="s">
         <v>146</v>
       </c>
@@ -5275,8 +5275,8 @@
       <c r="N57" s="25"/>
     </row>
     <row r="58" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="228"/>
-      <c r="B58" s="254" t="s">
+      <c r="A58" s="217"/>
+      <c r="B58" s="216" t="s">
         <v>147</v>
       </c>
       <c r="C58" s="157" t="s">
@@ -5295,8 +5295,8 @@
       <c r="N58" s="25"/>
     </row>
     <row r="59" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="228"/>
-      <c r="B59" s="254"/>
+      <c r="A59" s="217"/>
+      <c r="B59" s="216"/>
       <c r="C59" s="157" t="s">
         <v>106</v>
       </c>
@@ -5313,8 +5313,8 @@
       <c r="N59" s="25"/>
     </row>
     <row r="60" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="228"/>
-      <c r="B60" s="253" t="s">
+      <c r="A60" s="217"/>
+      <c r="B60" s="215" t="s">
         <v>149</v>
       </c>
       <c r="C60" s="13" t="s">
@@ -5333,8 +5333,8 @@
       <c r="N60" s="8"/>
     </row>
     <row r="61" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="228"/>
-      <c r="B61" s="253"/>
+      <c r="A61" s="217"/>
+      <c r="B61" s="215"/>
       <c r="C61" s="153" t="s">
         <v>150</v>
       </c>
@@ -5351,8 +5351,8 @@
       <c r="N61" s="25"/>
     </row>
     <row r="62" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="228"/>
-      <c r="B62" s="253" t="s">
+      <c r="A62" s="217"/>
+      <c r="B62" s="215" t="s">
         <v>151</v>
       </c>
       <c r="C62" s="154" t="s">
@@ -5371,8 +5371,8 @@
       <c r="N62" s="25"/>
     </row>
     <row r="63" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="229"/>
-      <c r="B63" s="257"/>
+      <c r="A63" s="218"/>
+      <c r="B63" s="222"/>
       <c r="C63" s="155" t="s">
         <v>106</v>
       </c>
@@ -5389,11 +5389,11 @@
       <c r="N63" s="26"/>
     </row>
     <row r="64" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="222" t="s">
+      <c r="A64" s="243" t="s">
         <v>153</v>
       </c>
-      <c r="B64" s="222"/>
-      <c r="C64" s="222"/>
+      <c r="B64" s="243"/>
+      <c r="C64" s="243"/>
       <c r="D64" s="73"/>
       <c r="E64" s="16"/>
       <c r="F64" s="16"/>
@@ -5407,11 +5407,11 @@
       <c r="N64" s="40"/>
     </row>
     <row r="65" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="237" t="s">
+      <c r="A65" s="239" t="s">
         <v>154</v>
       </c>
-      <c r="B65" s="237"/>
-      <c r="C65" s="237"/>
+      <c r="B65" s="239"/>
+      <c r="C65" s="239"/>
       <c r="D65" s="70"/>
       <c r="E65" s="42"/>
       <c r="F65" s="42"/>
@@ -5425,10 +5425,10 @@
       <c r="N65" s="42"/>
     </row>
     <row r="66" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="228" t="s">
+      <c r="A66" s="217" t="s">
         <v>155</v>
       </c>
-      <c r="B66" s="221" t="s">
+      <c r="B66" s="213" t="s">
         <v>156</v>
       </c>
       <c r="C66" s="43" t="s">
@@ -5447,8 +5447,8 @@
       <c r="N66" s="44"/>
     </row>
     <row r="67" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="228"/>
-      <c r="B67" s="221"/>
+      <c r="A67" s="217"/>
+      <c r="B67" s="213"/>
       <c r="C67" s="153" t="s">
         <v>157</v>
       </c>
@@ -5465,8 +5465,8 @@
       <c r="N67" s="24"/>
     </row>
     <row r="68" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="228"/>
-      <c r="B68" s="221"/>
+      <c r="A68" s="217"/>
+      <c r="B68" s="213"/>
       <c r="C68" s="154" t="s">
         <v>158</v>
       </c>
@@ -5483,8 +5483,8 @@
       <c r="N68" s="25"/>
     </row>
     <row r="69" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="228"/>
-      <c r="B69" s="221"/>
+      <c r="A69" s="217"/>
+      <c r="B69" s="213"/>
       <c r="C69" s="154" t="s">
         <v>159</v>
       </c>
@@ -5501,8 +5501,8 @@
       <c r="N69" s="25"/>
     </row>
     <row r="70" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="228"/>
-      <c r="B70" s="221"/>
+      <c r="A70" s="217"/>
+      <c r="B70" s="213"/>
       <c r="C70" s="154" t="s">
         <v>160</v>
       </c>
@@ -5519,8 +5519,8 @@
       <c r="N70" s="25"/>
     </row>
     <row r="71" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="228"/>
-      <c r="B71" s="221"/>
+      <c r="A71" s="217"/>
+      <c r="B71" s="213"/>
       <c r="C71" s="154" t="s">
         <v>106</v>
       </c>
@@ -5537,8 +5537,8 @@
       <c r="N71" s="25"/>
     </row>
     <row r="72" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="228"/>
-      <c r="B72" s="221"/>
+      <c r="A72" s="217"/>
+      <c r="B72" s="213"/>
       <c r="C72" s="13" t="s">
         <v>85</v>
       </c>
@@ -5555,8 +5555,8 @@
       <c r="N72" s="8"/>
     </row>
     <row r="73" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="228"/>
-      <c r="B73" s="221"/>
+      <c r="A73" s="217"/>
+      <c r="B73" s="213"/>
       <c r="C73" s="153" t="s">
         <v>161</v>
       </c>
@@ -5573,8 +5573,8 @@
       <c r="N73" s="25"/>
     </row>
     <row r="74" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="228"/>
-      <c r="B74" s="224"/>
+      <c r="A74" s="217"/>
+      <c r="B74" s="214"/>
       <c r="C74" s="155" t="s">
         <v>106</v>
       </c>
@@ -5591,8 +5591,8 @@
       <c r="N74" s="26"/>
     </row>
     <row r="75" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="228"/>
-      <c r="B75" s="223" t="s">
+      <c r="A75" s="217"/>
+      <c r="B75" s="212" t="s">
         <v>162</v>
       </c>
       <c r="C75" s="13" t="s">
@@ -5611,8 +5611,8 @@
       <c r="N75" s="8"/>
     </row>
     <row r="76" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="228"/>
-      <c r="B76" s="221"/>
+      <c r="A76" s="217"/>
+      <c r="B76" s="213"/>
       <c r="C76" s="153" t="s">
         <v>163</v>
       </c>
@@ -5629,8 +5629,8 @@
       <c r="N76" s="24"/>
     </row>
     <row r="77" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="228"/>
-      <c r="B77" s="221"/>
+      <c r="A77" s="217"/>
+      <c r="B77" s="213"/>
       <c r="C77" s="154" t="s">
         <v>164</v>
       </c>
@@ -5647,8 +5647,8 @@
       <c r="N77" s="25"/>
     </row>
     <row r="78" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="228"/>
-      <c r="B78" s="221"/>
+      <c r="A78" s="217"/>
+      <c r="B78" s="213"/>
       <c r="C78" s="13" t="s">
         <v>85</v>
       </c>
@@ -5665,8 +5665,8 @@
       <c r="N78" s="8"/>
     </row>
     <row r="79" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="228"/>
-      <c r="B79" s="221"/>
+      <c r="A79" s="217"/>
+      <c r="B79" s="213"/>
       <c r="C79" s="153" t="s">
         <v>165</v>
       </c>
@@ -5683,8 +5683,8 @@
       <c r="N79" s="25"/>
     </row>
     <row r="80" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="228"/>
-      <c r="B80" s="224"/>
+      <c r="A80" s="217"/>
+      <c r="B80" s="214"/>
       <c r="C80" s="155" t="s">
         <v>106</v>
       </c>
@@ -5701,8 +5701,8 @@
       <c r="N80" s="26"/>
     </row>
     <row r="81" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="228"/>
-      <c r="B81" s="223" t="s">
+      <c r="A81" s="217"/>
+      <c r="B81" s="212" t="s">
         <v>166</v>
       </c>
       <c r="C81" s="13" t="s">
@@ -5721,8 +5721,8 @@
       <c r="N81" s="8"/>
     </row>
     <row r="82" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="228"/>
-      <c r="B82" s="221"/>
+      <c r="A82" s="217"/>
+      <c r="B82" s="213"/>
       <c r="C82" s="153" t="s">
         <v>167</v>
       </c>
@@ -5739,8 +5739,8 @@
       <c r="N82" s="24"/>
     </row>
     <row r="83" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="228"/>
-      <c r="B83" s="221"/>
+      <c r="A83" s="217"/>
+      <c r="B83" s="213"/>
       <c r="C83" s="154" t="s">
         <v>168</v>
       </c>
@@ -5757,8 +5757,8 @@
       <c r="N83" s="25"/>
     </row>
     <row r="84" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="228"/>
-      <c r="B84" s="221"/>
+      <c r="A84" s="217"/>
+      <c r="B84" s="213"/>
       <c r="C84" s="154" t="s">
         <v>169</v>
       </c>
@@ -5775,8 +5775,8 @@
       <c r="N84" s="25"/>
     </row>
     <row r="85" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="228"/>
-      <c r="B85" s="221"/>
+      <c r="A85" s="217"/>
+      <c r="B85" s="213"/>
       <c r="C85" s="154" t="s">
         <v>106</v>
       </c>
@@ -5793,8 +5793,8 @@
       <c r="N85" s="25"/>
     </row>
     <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="228"/>
-      <c r="B86" s="221"/>
+      <c r="A86" s="217"/>
+      <c r="B86" s="213"/>
       <c r="C86" s="13" t="s">
         <v>85</v>
       </c>
@@ -5811,8 +5811,8 @@
       <c r="N86" s="8"/>
     </row>
     <row r="87" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="228"/>
-      <c r="B87" s="221"/>
+      <c r="A87" s="217"/>
+      <c r="B87" s="213"/>
       <c r="C87" s="153" t="s">
         <v>170</v>
       </c>
@@ -5829,8 +5829,8 @@
       <c r="N87" s="25"/>
     </row>
     <row r="88" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="229"/>
-      <c r="B88" s="224"/>
+      <c r="A88" s="218"/>
+      <c r="B88" s="214"/>
       <c r="C88" s="155" t="s">
         <v>171</v>
       </c>
@@ -5847,11 +5847,11 @@
       <c r="N88" s="26"/>
     </row>
     <row r="89" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="230" t="s">
+      <c r="A89" s="223" t="s">
         <v>172</v>
       </c>
-      <c r="B89" s="230"/>
-      <c r="C89" s="230"/>
+      <c r="B89" s="223"/>
+      <c r="C89" s="223"/>
       <c r="D89" s="70"/>
       <c r="E89" s="42"/>
       <c r="F89" s="42"/>
@@ -5865,10 +5865,10 @@
       <c r="N89" s="42"/>
     </row>
     <row r="90" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="228" t="s">
+      <c r="A90" s="217" t="s">
         <v>173</v>
       </c>
-      <c r="B90" s="221" t="s">
+      <c r="B90" s="213" t="s">
         <v>174</v>
       </c>
       <c r="C90" s="43" t="s">
@@ -5887,8 +5887,8 @@
       <c r="N90" s="44"/>
     </row>
     <row r="91" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="228"/>
-      <c r="B91" s="221"/>
+      <c r="A91" s="217"/>
+      <c r="B91" s="213"/>
       <c r="C91" s="153" t="s">
         <v>175</v>
       </c>
@@ -5905,8 +5905,8 @@
       <c r="N91" s="24"/>
     </row>
     <row r="92" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="228"/>
-      <c r="B92" s="221"/>
+      <c r="A92" s="217"/>
+      <c r="B92" s="213"/>
       <c r="C92" s="154" t="s">
         <v>176</v>
       </c>
@@ -5923,8 +5923,8 @@
       <c r="N92" s="25"/>
     </row>
     <row r="93" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="228"/>
-      <c r="B93" s="221"/>
+      <c r="A93" s="217"/>
+      <c r="B93" s="213"/>
       <c r="C93" s="154" t="s">
         <v>177</v>
       </c>
@@ -5941,8 +5941,8 @@
       <c r="N93" s="25"/>
     </row>
     <row r="94" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="228"/>
-      <c r="B94" s="221"/>
+      <c r="A94" s="217"/>
+      <c r="B94" s="213"/>
       <c r="C94" s="154" t="s">
         <v>178</v>
       </c>
@@ -5959,8 +5959,8 @@
       <c r="N94" s="25"/>
     </row>
     <row r="95" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="228"/>
-      <c r="B95" s="221"/>
+      <c r="A95" s="217"/>
+      <c r="B95" s="213"/>
       <c r="C95" s="154" t="s">
         <v>106</v>
       </c>
@@ -5977,8 +5977,8 @@
       <c r="N95" s="25"/>
     </row>
     <row r="96" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="228"/>
-      <c r="B96" s="221"/>
+      <c r="A96" s="217"/>
+      <c r="B96" s="213"/>
       <c r="C96" s="13" t="s">
         <v>85</v>
       </c>
@@ -5995,8 +5995,8 @@
       <c r="N96" s="8"/>
     </row>
     <row r="97" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="228"/>
-      <c r="B97" s="221"/>
+      <c r="A97" s="217"/>
+      <c r="B97" s="213"/>
       <c r="C97" s="153" t="s">
         <v>179</v>
       </c>
@@ -6013,8 +6013,8 @@
       <c r="N97" s="25"/>
     </row>
     <row r="98" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="228"/>
-      <c r="B98" s="221"/>
+      <c r="A98" s="217"/>
+      <c r="B98" s="213"/>
       <c r="C98" s="154" t="s">
         <v>180</v>
       </c>
@@ -6031,8 +6031,8 @@
       <c r="N98" s="25"/>
     </row>
     <row r="99" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="228"/>
-      <c r="B99" s="221"/>
+      <c r="A99" s="217"/>
+      <c r="B99" s="213"/>
       <c r="C99" s="154" t="s">
         <v>181</v>
       </c>
@@ -6049,8 +6049,8 @@
       <c r="N99" s="25"/>
     </row>
     <row r="100" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="228"/>
-      <c r="B100" s="221"/>
+      <c r="A100" s="217"/>
+      <c r="B100" s="213"/>
       <c r="C100" s="154" t="s">
         <v>182</v>
       </c>
@@ -6067,8 +6067,8 @@
       <c r="N100" s="25"/>
     </row>
     <row r="101" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="229"/>
-      <c r="B101" s="224"/>
+      <c r="A101" s="218"/>
+      <c r="B101" s="214"/>
       <c r="C101" s="155" t="s">
         <v>106</v>
       </c>
@@ -6085,11 +6085,11 @@
       <c r="N101" s="26"/>
     </row>
     <row r="102" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="230" t="s">
+      <c r="A102" s="223" t="s">
         <v>183</v>
       </c>
-      <c r="B102" s="230"/>
-      <c r="C102" s="230"/>
+      <c r="B102" s="223"/>
+      <c r="C102" s="223"/>
       <c r="D102" s="70"/>
       <c r="E102" s="42"/>
       <c r="F102" s="42"/>
@@ -6103,10 +6103,10 @@
       <c r="N102" s="42"/>
     </row>
     <row r="103" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="228" t="s">
+      <c r="A103" s="217" t="s">
         <v>184</v>
       </c>
-      <c r="B103" s="221" t="s">
+      <c r="B103" s="213" t="s">
         <v>185</v>
       </c>
       <c r="C103" s="43" t="s">
@@ -6125,8 +6125,8 @@
       <c r="N103" s="44"/>
     </row>
     <row r="104" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="228"/>
-      <c r="B104" s="221"/>
+      <c r="A104" s="217"/>
+      <c r="B104" s="213"/>
       <c r="C104" s="153" t="s">
         <v>186</v>
       </c>
@@ -6143,8 +6143,8 @@
       <c r="N104" s="25"/>
     </row>
     <row r="105" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="228"/>
-      <c r="B105" s="221"/>
+      <c r="A105" s="217"/>
+      <c r="B105" s="213"/>
       <c r="C105" s="154" t="s">
         <v>187</v>
       </c>
@@ -6161,8 +6161,8 @@
       <c r="N105" s="25"/>
     </row>
     <row r="106" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="228"/>
-      <c r="B106" s="221"/>
+      <c r="A106" s="217"/>
+      <c r="B106" s="213"/>
       <c r="C106" s="154" t="s">
         <v>188</v>
       </c>
@@ -6179,8 +6179,8 @@
       <c r="N106" s="25"/>
     </row>
     <row r="107" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="228"/>
-      <c r="B107" s="221"/>
+      <c r="A107" s="217"/>
+      <c r="B107" s="213"/>
       <c r="C107" s="154" t="s">
         <v>189</v>
       </c>
@@ -6197,8 +6197,8 @@
       <c r="N107" s="25"/>
     </row>
     <row r="108" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="228"/>
-      <c r="B108" s="221"/>
+      <c r="A108" s="217"/>
+      <c r="B108" s="213"/>
       <c r="C108" s="154" t="s">
         <v>190</v>
       </c>
@@ -6215,8 +6215,8 @@
       <c r="N108" s="25"/>
     </row>
     <row r="109" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="228"/>
-      <c r="B109" s="221"/>
+      <c r="A109" s="217"/>
+      <c r="B109" s="213"/>
       <c r="C109" s="154" t="s">
         <v>106</v>
       </c>
@@ -6233,8 +6233,8 @@
       <c r="N109" s="25"/>
     </row>
     <row r="110" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="228"/>
-      <c r="B110" s="221"/>
+      <c r="A110" s="217"/>
+      <c r="B110" s="213"/>
       <c r="C110" s="13" t="s">
         <v>85</v>
       </c>
@@ -6251,8 +6251,8 @@
       <c r="N110" s="8"/>
     </row>
     <row r="111" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="228"/>
-      <c r="B111" s="221"/>
+      <c r="A111" s="217"/>
+      <c r="B111" s="213"/>
       <c r="C111" s="153" t="s">
         <v>191</v>
       </c>
@@ -6269,8 +6269,8 @@
       <c r="N111" s="25"/>
     </row>
     <row r="112" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="228"/>
-      <c r="B112" s="221"/>
+      <c r="A112" s="217"/>
+      <c r="B112" s="213"/>
       <c r="C112" s="154" t="s">
         <v>192</v>
       </c>
@@ -6287,8 +6287,8 @@
       <c r="N112" s="25"/>
     </row>
     <row r="113" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="228"/>
-      <c r="B113" s="224"/>
+      <c r="A113" s="217"/>
+      <c r="B113" s="214"/>
       <c r="C113" s="155" t="s">
         <v>193</v>
       </c>
@@ -6305,8 +6305,8 @@
       <c r="N113" s="26"/>
     </row>
     <row r="114" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="228"/>
-      <c r="B114" s="223" t="s">
+      <c r="A114" s="217"/>
+      <c r="B114" s="212" t="s">
         <v>194</v>
       </c>
       <c r="C114" s="13" t="s">
@@ -6325,8 +6325,8 @@
       <c r="N114" s="8"/>
     </row>
     <row r="115" spans="1:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="228"/>
-      <c r="B115" s="221"/>
+      <c r="A115" s="217"/>
+      <c r="B115" s="213"/>
       <c r="C115" s="153" t="s">
         <v>195</v>
       </c>
@@ -6343,8 +6343,8 @@
       <c r="N115" s="25"/>
     </row>
     <row r="116" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="228"/>
-      <c r="B116" s="221"/>
+      <c r="A116" s="217"/>
+      <c r="B116" s="213"/>
       <c r="C116" s="154" t="s">
         <v>106</v>
       </c>
@@ -6361,8 +6361,8 @@
       <c r="N116" s="25"/>
     </row>
     <row r="117" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="228"/>
-      <c r="B117" s="221"/>
+      <c r="A117" s="217"/>
+      <c r="B117" s="213"/>
       <c r="C117" s="13" t="s">
         <v>85</v>
       </c>
@@ -6379,8 +6379,8 @@
       <c r="N117" s="8"/>
     </row>
     <row r="118" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="228"/>
-      <c r="B118" s="221"/>
+      <c r="A118" s="217"/>
+      <c r="B118" s="213"/>
       <c r="C118" s="153" t="s">
         <v>196</v>
       </c>
@@ -6397,8 +6397,8 @@
       <c r="N118" s="25"/>
     </row>
     <row r="119" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="229"/>
-      <c r="B119" s="224"/>
+      <c r="A119" s="218"/>
+      <c r="B119" s="214"/>
       <c r="C119" s="155" t="s">
         <v>193</v>
       </c>
@@ -6415,11 +6415,11 @@
       <c r="N119" s="26"/>
     </row>
     <row r="120" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="230" t="s">
+      <c r="A120" s="223" t="s">
         <v>197</v>
       </c>
-      <c r="B120" s="230"/>
-      <c r="C120" s="230"/>
+      <c r="B120" s="223"/>
+      <c r="C120" s="223"/>
       <c r="D120" s="70"/>
       <c r="E120" s="42"/>
       <c r="F120" s="42"/>
@@ -6433,10 +6433,10 @@
       <c r="N120" s="45"/>
     </row>
     <row r="121" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="228" t="s">
+      <c r="A121" s="217" t="s">
         <v>198</v>
       </c>
-      <c r="B121" s="221" t="s">
+      <c r="B121" s="213" t="s">
         <v>199</v>
       </c>
       <c r="C121" s="43" t="s">
@@ -6455,8 +6455,8 @@
       <c r="N121" s="44"/>
     </row>
     <row r="122" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="228"/>
-      <c r="B122" s="221"/>
+      <c r="A122" s="217"/>
+      <c r="B122" s="213"/>
       <c r="C122" s="154" t="s">
         <v>200</v>
       </c>
@@ -6473,8 +6473,8 @@
       <c r="N122" s="25"/>
     </row>
     <row r="123" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="228"/>
-      <c r="B123" s="221"/>
+      <c r="A123" s="217"/>
+      <c r="B123" s="213"/>
       <c r="C123" s="154" t="s">
         <v>201</v>
       </c>
@@ -6491,7 +6491,7 @@
       <c r="N123" s="25"/>
     </row>
     <row r="124" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="228"/>
+      <c r="A124" s="217"/>
       <c r="B124" s="33" t="s">
         <v>111</v>
       </c>
@@ -6511,8 +6511,8 @@
       <c r="N124" s="25"/>
     </row>
     <row r="125" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="228"/>
-      <c r="B125" s="212" t="s">
+      <c r="A125" s="217"/>
+      <c r="B125" s="221" t="s">
         <v>203</v>
       </c>
       <c r="C125" s="154" t="s">
@@ -6531,8 +6531,8 @@
       <c r="N125" s="25"/>
     </row>
     <row r="126" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="228"/>
-      <c r="B126" s="212"/>
+      <c r="A126" s="217"/>
+      <c r="B126" s="221"/>
       <c r="C126" s="13" t="s">
         <v>85</v>
       </c>
@@ -6549,8 +6549,8 @@
       <c r="N126" s="8"/>
     </row>
     <row r="127" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="228"/>
-      <c r="B127" s="212"/>
+      <c r="A127" s="217"/>
+      <c r="B127" s="221"/>
       <c r="C127" s="153" t="s">
         <v>204</v>
       </c>
@@ -6567,7 +6567,7 @@
       <c r="N127" s="25"/>
     </row>
     <row r="128" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="228"/>
+      <c r="A128" s="217"/>
       <c r="B128" s="32" t="s">
         <v>205</v>
       </c>
@@ -6587,8 +6587,8 @@
       <c r="N128" s="28"/>
     </row>
     <row r="129" spans="1:14" s="186" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="228"/>
-      <c r="B129" s="223" t="s">
+      <c r="A129" s="217"/>
+      <c r="B129" s="212" t="s">
         <v>206</v>
       </c>
       <c r="C129" s="90" t="s">
@@ -6607,8 +6607,8 @@
       <c r="N129" s="81"/>
     </row>
     <row r="130" spans="1:14" s="187" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="228"/>
-      <c r="B130" s="221"/>
+      <c r="A130" s="217"/>
+      <c r="B130" s="213"/>
       <c r="C130" s="158" t="s">
         <v>207</v>
       </c>
@@ -6625,8 +6625,8 @@
       <c r="N130" s="84"/>
     </row>
     <row r="131" spans="1:14" s="187" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="228"/>
-      <c r="B131" s="221"/>
+      <c r="A131" s="217"/>
+      <c r="B131" s="213"/>
       <c r="C131" s="159" t="s">
         <v>208</v>
       </c>
@@ -6643,8 +6643,8 @@
       <c r="N131" s="79"/>
     </row>
     <row r="132" spans="1:14" s="187" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="228"/>
-      <c r="B132" s="221"/>
+      <c r="A132" s="217"/>
+      <c r="B132" s="213"/>
       <c r="C132" s="160" t="s">
         <v>209</v>
       </c>
@@ -6661,8 +6661,8 @@
       <c r="N132" s="79"/>
     </row>
     <row r="133" spans="1:14" s="188" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="228"/>
-      <c r="B133" s="221"/>
+      <c r="A133" s="217"/>
+      <c r="B133" s="213"/>
       <c r="C133" s="161" t="s">
         <v>210</v>
       </c>
@@ -6679,8 +6679,8 @@
       <c r="N133" s="80"/>
     </row>
     <row r="134" spans="1:14" s="188" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="228"/>
-      <c r="B134" s="221"/>
+      <c r="A134" s="217"/>
+      <c r="B134" s="213"/>
       <c r="C134" s="161" t="s">
         <v>211</v>
       </c>
@@ -6697,8 +6697,8 @@
       <c r="N134" s="80"/>
     </row>
     <row r="135" spans="1:14" s="188" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="228"/>
-      <c r="B135" s="221"/>
+      <c r="A135" s="217"/>
+      <c r="B135" s="213"/>
       <c r="C135" s="162" t="s">
         <v>106</v>
       </c>
@@ -6715,8 +6715,8 @@
       <c r="N135" s="80"/>
     </row>
     <row r="136" spans="1:14" s="186" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="228"/>
-      <c r="B136" s="221"/>
+      <c r="A136" s="217"/>
+      <c r="B136" s="213"/>
       <c r="C136" s="83" t="s">
         <v>85</v>
       </c>
@@ -6733,8 +6733,8 @@
       <c r="N136" s="81"/>
     </row>
     <row r="137" spans="1:14" s="187" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="228"/>
-      <c r="B137" s="221"/>
+      <c r="A137" s="217"/>
+      <c r="B137" s="213"/>
       <c r="C137" s="158" t="s">
         <v>212</v>
       </c>
@@ -6751,8 +6751,8 @@
       <c r="N137" s="84"/>
     </row>
     <row r="138" spans="1:14" s="187" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="228"/>
-      <c r="B138" s="221"/>
+      <c r="A138" s="217"/>
+      <c r="B138" s="213"/>
       <c r="C138" s="154" t="s">
         <v>213</v>
       </c>
@@ -6769,8 +6769,8 @@
       <c r="N138" s="79"/>
     </row>
     <row r="139" spans="1:14" s="187" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="228"/>
-      <c r="B139" s="221"/>
+      <c r="A139" s="217"/>
+      <c r="B139" s="213"/>
       <c r="C139" s="161" t="s">
         <v>214</v>
       </c>
@@ -6787,8 +6787,8 @@
       <c r="N139" s="74"/>
     </row>
     <row r="140" spans="1:14" s="187" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="229"/>
-      <c r="B140" s="224"/>
+      <c r="A140" s="218"/>
+      <c r="B140" s="214"/>
       <c r="C140" s="163" t="s">
         <v>106</v>
       </c>
@@ -6805,11 +6805,11 @@
       <c r="N140" s="88"/>
     </row>
     <row r="141" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="230" t="s">
+      <c r="A141" s="223" t="s">
         <v>215</v>
       </c>
-      <c r="B141" s="230"/>
-      <c r="C141" s="230"/>
+      <c r="B141" s="223"/>
+      <c r="C141" s="223"/>
       <c r="D141" s="75"/>
       <c r="E141" s="66"/>
       <c r="F141" s="66"/>
@@ -6823,10 +6823,10 @@
       <c r="N141" s="66"/>
     </row>
     <row r="142" spans="1:14" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="228" t="s">
+      <c r="A142" s="217" t="s">
         <v>216</v>
       </c>
-      <c r="B142" s="221" t="s">
+      <c r="B142" s="213" t="s">
         <v>217</v>
       </c>
       <c r="C142" s="43" t="s">
@@ -6845,8 +6845,8 @@
       <c r="N142" s="44"/>
     </row>
     <row r="143" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="228"/>
-      <c r="B143" s="221"/>
+      <c r="A143" s="217"/>
+      <c r="B143" s="213"/>
       <c r="C143" s="153" t="s">
         <v>218</v>
       </c>
@@ -6863,7 +6863,7 @@
       <c r="N143" s="25"/>
     </row>
     <row r="144" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="228"/>
+      <c r="A144" s="217"/>
       <c r="B144" s="33" t="s">
         <v>141</v>
       </c>
@@ -6883,8 +6883,8 @@
       <c r="N144" s="25"/>
     </row>
     <row r="145" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="228"/>
-      <c r="B145" s="212" t="s">
+      <c r="A145" s="217"/>
+      <c r="B145" s="221" t="s">
         <v>220</v>
       </c>
       <c r="C145" s="154" t="s">
@@ -6903,8 +6903,8 @@
       <c r="N145" s="25"/>
     </row>
     <row r="146" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="228"/>
-      <c r="B146" s="212"/>
+      <c r="A146" s="217"/>
+      <c r="B146" s="221"/>
       <c r="C146" s="154" t="s">
         <v>222</v>
       </c>
@@ -6921,8 +6921,8 @@
       <c r="N146" s="25"/>
     </row>
     <row r="147" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="228"/>
-      <c r="B147" s="212"/>
+      <c r="A147" s="217"/>
+      <c r="B147" s="221"/>
       <c r="C147" s="154" t="s">
         <v>223</v>
       </c>
@@ -6939,8 +6939,8 @@
       <c r="N147" s="25"/>
     </row>
     <row r="148" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="228"/>
-      <c r="B148" s="255" t="s">
+      <c r="A148" s="217"/>
+      <c r="B148" s="219" t="s">
         <v>224</v>
       </c>
       <c r="C148" s="154" t="s">
@@ -6959,8 +6959,8 @@
       <c r="N148" s="25"/>
     </row>
     <row r="149" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="228"/>
-      <c r="B149" s="255"/>
+      <c r="A149" s="217"/>
+      <c r="B149" s="219"/>
       <c r="C149" s="154" t="s">
         <v>106</v>
       </c>
@@ -6977,8 +6977,8 @@
       <c r="N149" s="25"/>
     </row>
     <row r="150" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="228"/>
-      <c r="B150" s="255"/>
+      <c r="A150" s="217"/>
+      <c r="B150" s="219"/>
       <c r="C150" s="13" t="s">
         <v>85</v>
       </c>
@@ -6995,8 +6995,8 @@
       <c r="N150" s="8"/>
     </row>
     <row r="151" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="228"/>
-      <c r="B151" s="255"/>
+      <c r="A151" s="217"/>
+      <c r="B151" s="219"/>
       <c r="C151" s="153" t="s">
         <v>226</v>
       </c>
@@ -7013,8 +7013,8 @@
       <c r="N151" s="25"/>
     </row>
     <row r="152" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="228"/>
-      <c r="B152" s="256"/>
+      <c r="A152" s="217"/>
+      <c r="B152" s="220"/>
       <c r="C152" s="155" t="s">
         <v>106</v>
       </c>
@@ -7031,8 +7031,8 @@
       <c r="N152" s="26"/>
     </row>
     <row r="153" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="228"/>
-      <c r="B153" s="223" t="s">
+      <c r="A153" s="217"/>
+      <c r="B153" s="212" t="s">
         <v>227</v>
       </c>
       <c r="C153" s="13" t="s">
@@ -7051,8 +7051,8 @@
       <c r="N153" s="8"/>
     </row>
     <row r="154" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="228"/>
-      <c r="B154" s="221"/>
+      <c r="A154" s="217"/>
+      <c r="B154" s="213"/>
       <c r="C154" s="153" t="s">
         <v>228</v>
       </c>
@@ -7069,7 +7069,7 @@
       <c r="N154" s="25"/>
     </row>
     <row r="155" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="228"/>
+      <c r="A155" s="217"/>
       <c r="B155" s="33" t="s">
         <v>111</v>
       </c>
@@ -7089,8 +7089,8 @@
       <c r="N155" s="25"/>
     </row>
     <row r="156" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="228"/>
-      <c r="B156" s="212" t="s">
+      <c r="A156" s="217"/>
+      <c r="B156" s="221" t="s">
         <v>230</v>
       </c>
       <c r="C156" s="154" t="s">
@@ -7109,8 +7109,8 @@
       <c r="N156" s="25"/>
     </row>
     <row r="157" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="228"/>
-      <c r="B157" s="212"/>
+      <c r="A157" s="217"/>
+      <c r="B157" s="221"/>
       <c r="C157" s="154" t="s">
         <v>106</v>
       </c>
@@ -7127,8 +7127,8 @@
       <c r="N157" s="25"/>
     </row>
     <row r="158" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="228"/>
-      <c r="B158" s="212"/>
+      <c r="A158" s="217"/>
+      <c r="B158" s="221"/>
       <c r="C158" s="13" t="s">
         <v>85</v>
       </c>
@@ -7145,8 +7145,8 @@
       <c r="N158" s="8"/>
     </row>
     <row r="159" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="228"/>
-      <c r="B159" s="212"/>
+      <c r="A159" s="217"/>
+      <c r="B159" s="221"/>
       <c r="C159" s="153" t="s">
         <v>232</v>
       </c>
@@ -7163,8 +7163,8 @@
       <c r="N159" s="25"/>
     </row>
     <row r="160" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="228"/>
-      <c r="B160" s="212"/>
+      <c r="A160" s="217"/>
+      <c r="B160" s="221"/>
       <c r="C160" s="34" t="s">
         <v>233</v>
       </c>
@@ -7181,8 +7181,8 @@
       <c r="N160" s="28"/>
     </row>
     <row r="161" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="228"/>
-      <c r="B161" s="213"/>
+      <c r="A161" s="217"/>
+      <c r="B161" s="236"/>
       <c r="C161" s="155" t="s">
         <v>106</v>
       </c>
@@ -7199,8 +7199,8 @@
       <c r="N161" s="26"/>
     </row>
     <row r="162" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="228"/>
-      <c r="B162" s="223" t="s">
+      <c r="A162" s="217"/>
+      <c r="B162" s="212" t="s">
         <v>234</v>
       </c>
       <c r="C162" s="13" t="s">
@@ -7219,8 +7219,8 @@
       <c r="N162" s="8"/>
     </row>
     <row r="163" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="228"/>
-      <c r="B163" s="221"/>
+      <c r="A163" s="217"/>
+      <c r="B163" s="213"/>
       <c r="C163" s="153" t="s">
         <v>235</v>
       </c>
@@ -7237,7 +7237,7 @@
       <c r="N163" s="25"/>
     </row>
     <row r="164" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="228"/>
+      <c r="A164" s="217"/>
       <c r="B164" s="33" t="s">
         <v>111</v>
       </c>
@@ -7257,7 +7257,7 @@
       <c r="N164" s="25"/>
     </row>
     <row r="165" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="228"/>
+      <c r="A165" s="217"/>
       <c r="B165" s="32" t="s">
         <v>237</v>
       </c>
@@ -7277,8 +7277,8 @@
       <c r="N165" s="25"/>
     </row>
     <row r="166" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="228"/>
-      <c r="B166" s="212" t="s">
+      <c r="A166" s="217"/>
+      <c r="B166" s="221" t="s">
         <v>239</v>
       </c>
       <c r="C166" s="154" t="s">
@@ -7297,8 +7297,8 @@
       <c r="N166" s="25"/>
     </row>
     <row r="167" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="228"/>
-      <c r="B167" s="212"/>
+      <c r="A167" s="217"/>
+      <c r="B167" s="221"/>
       <c r="C167" s="154" t="s">
         <v>241</v>
       </c>
@@ -7315,8 +7315,8 @@
       <c r="N167" s="25"/>
     </row>
     <row r="168" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="228"/>
-      <c r="B168" s="212"/>
+      <c r="A168" s="217"/>
+      <c r="B168" s="221"/>
       <c r="C168" s="154" t="s">
         <v>242</v>
       </c>
@@ -7333,8 +7333,8 @@
       <c r="N168" s="25"/>
     </row>
     <row r="169" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="228"/>
-      <c r="B169" s="212"/>
+      <c r="A169" s="217"/>
+      <c r="B169" s="221"/>
       <c r="C169" s="154" t="s">
         <v>106</v>
       </c>
@@ -7351,8 +7351,8 @@
       <c r="N169" s="25"/>
     </row>
     <row r="170" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="228"/>
-      <c r="B170" s="212"/>
+      <c r="A170" s="217"/>
+      <c r="B170" s="221"/>
       <c r="C170" s="13" t="s">
         <v>85</v>
       </c>
@@ -7369,8 +7369,8 @@
       <c r="N170" s="8"/>
     </row>
     <row r="171" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="228"/>
-      <c r="B171" s="212"/>
+      <c r="A171" s="217"/>
+      <c r="B171" s="221"/>
       <c r="C171" s="153" t="s">
         <v>243</v>
       </c>
@@ -7387,8 +7387,8 @@
       <c r="N171" s="25"/>
     </row>
     <row r="172" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="228"/>
-      <c r="B172" s="212"/>
+      <c r="A172" s="217"/>
+      <c r="B172" s="221"/>
       <c r="C172" s="154" t="s">
         <v>244</v>
       </c>
@@ -7405,8 +7405,8 @@
       <c r="N172" s="25"/>
     </row>
     <row r="173" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="228"/>
-      <c r="B173" s="213"/>
+      <c r="A173" s="217"/>
+      <c r="B173" s="236"/>
       <c r="C173" s="155" t="s">
         <v>106</v>
       </c>
@@ -7423,8 +7423,8 @@
       <c r="N173" s="26"/>
     </row>
     <row r="174" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="228"/>
-      <c r="B174" s="223" t="s">
+      <c r="A174" s="217"/>
+      <c r="B174" s="212" t="s">
         <v>245</v>
       </c>
       <c r="C174" s="13" t="s">
@@ -7443,8 +7443,8 @@
       <c r="N174" s="8"/>
     </row>
     <row r="175" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="228"/>
-      <c r="B175" s="221"/>
+      <c r="A175" s="217"/>
+      <c r="B175" s="213"/>
       <c r="C175" s="153" t="s">
         <v>247</v>
       </c>
@@ -7461,8 +7461,8 @@
       <c r="N175" s="25"/>
     </row>
     <row r="176" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="228"/>
-      <c r="B176" s="221"/>
+      <c r="A176" s="217"/>
+      <c r="B176" s="213"/>
       <c r="C176" s="153" t="s">
         <v>248</v>
       </c>
@@ -7479,8 +7479,8 @@
       <c r="N176" s="25"/>
     </row>
     <row r="177" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="228"/>
-      <c r="B177" s="221"/>
+      <c r="A177" s="217"/>
+      <c r="B177" s="213"/>
       <c r="C177" s="154" t="s">
         <v>249</v>
       </c>
@@ -7497,8 +7497,8 @@
       <c r="N177" s="25"/>
     </row>
     <row r="178" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="228"/>
-      <c r="B178" s="221"/>
+      <c r="A178" s="217"/>
+      <c r="B178" s="213"/>
       <c r="C178" s="154" t="s">
         <v>250</v>
       </c>
@@ -7515,8 +7515,8 @@
       <c r="N178" s="25"/>
     </row>
     <row r="179" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="228"/>
-      <c r="B179" s="221"/>
+      <c r="A179" s="217"/>
+      <c r="B179" s="213"/>
       <c r="C179" s="154" t="s">
         <v>251</v>
       </c>
@@ -7533,8 +7533,8 @@
       <c r="N179" s="25"/>
     </row>
     <row r="180" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="228"/>
-      <c r="B180" s="221"/>
+      <c r="A180" s="217"/>
+      <c r="B180" s="213"/>
       <c r="C180" s="154" t="s">
         <v>252</v>
       </c>
@@ -7551,8 +7551,8 @@
       <c r="N180" s="25"/>
     </row>
     <row r="181" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="228"/>
-      <c r="B181" s="221"/>
+      <c r="A181" s="217"/>
+      <c r="B181" s="213"/>
       <c r="C181" s="154" t="s">
         <v>106</v>
       </c>
@@ -7569,8 +7569,8 @@
       <c r="N181" s="25"/>
     </row>
     <row r="182" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="228"/>
-      <c r="B182" s="221"/>
+      <c r="A182" s="217"/>
+      <c r="B182" s="213"/>
       <c r="C182" s="13" t="s">
         <v>85</v>
       </c>
@@ -7587,8 +7587,8 @@
       <c r="N182" s="8"/>
     </row>
     <row r="183" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="228"/>
-      <c r="B183" s="221"/>
+      <c r="A183" s="217"/>
+      <c r="B183" s="213"/>
       <c r="C183" s="153" t="s">
         <v>253</v>
       </c>
@@ -7605,8 +7605,8 @@
       <c r="N183" s="25"/>
     </row>
     <row r="184" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="229"/>
-      <c r="B184" s="224"/>
+      <c r="A184" s="218"/>
+      <c r="B184" s="214"/>
       <c r="C184" s="154" t="s">
         <v>106</v>
       </c>
@@ -7623,11 +7623,11 @@
       <c r="N184" s="10"/>
     </row>
     <row r="185" spans="1:14" s="185" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="230" t="s">
+      <c r="A185" s="223" t="s">
         <v>254</v>
       </c>
-      <c r="B185" s="230"/>
-      <c r="C185" s="230"/>
+      <c r="B185" s="223"/>
+      <c r="C185" s="223"/>
       <c r="D185" s="70"/>
       <c r="E185" s="42"/>
       <c r="F185" s="42"/>
@@ -7641,10 +7641,10 @@
       <c r="N185" s="45"/>
     </row>
     <row r="186" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="228" t="s">
+      <c r="A186" s="217" t="s">
         <v>255</v>
       </c>
-      <c r="B186" s="241" t="s">
+      <c r="B186" s="235" t="s">
         <v>256</v>
       </c>
       <c r="C186" s="43" t="s">
@@ -7663,8 +7663,8 @@
       <c r="N186" s="44"/>
     </row>
     <row r="187" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="228"/>
-      <c r="B187" s="241"/>
+      <c r="A187" s="217"/>
+      <c r="B187" s="235"/>
       <c r="C187" s="153" t="s">
         <v>257</v>
       </c>
@@ -7681,8 +7681,8 @@
       <c r="N187" s="25"/>
     </row>
     <row r="188" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="228"/>
-      <c r="B188" s="241"/>
+      <c r="A188" s="217"/>
+      <c r="B188" s="235"/>
       <c r="C188" s="154" t="s">
         <v>258</v>
       </c>
@@ -7699,8 +7699,8 @@
       <c r="N188" s="25"/>
     </row>
     <row r="189" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="228"/>
-      <c r="B189" s="241"/>
+      <c r="A189" s="217"/>
+      <c r="B189" s="235"/>
       <c r="C189" s="154" t="s">
         <v>259</v>
       </c>
@@ -7717,8 +7717,8 @@
       <c r="N189" s="25"/>
     </row>
     <row r="190" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="228"/>
-      <c r="B190" s="241"/>
+      <c r="A190" s="217"/>
+      <c r="B190" s="235"/>
       <c r="C190" s="154" t="s">
         <v>106</v>
       </c>
@@ -7735,8 +7735,8 @@
       <c r="N190" s="25"/>
     </row>
     <row r="191" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="228"/>
-      <c r="B191" s="241"/>
+      <c r="A191" s="217"/>
+      <c r="B191" s="235"/>
       <c r="C191" s="13" t="s">
         <v>85</v>
       </c>
@@ -7753,8 +7753,8 @@
       <c r="N191" s="8"/>
     </row>
     <row r="192" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="228"/>
-      <c r="B192" s="241"/>
+      <c r="A192" s="217"/>
+      <c r="B192" s="235"/>
       <c r="C192" s="153" t="s">
         <v>260</v>
       </c>
@@ -7771,8 +7771,8 @@
       <c r="N192" s="25"/>
     </row>
     <row r="193" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="228"/>
-      <c r="B193" s="241"/>
+      <c r="A193" s="217"/>
+      <c r="B193" s="235"/>
       <c r="C193" s="154" t="s">
         <v>261</v>
       </c>
@@ -7789,8 +7789,8 @@
       <c r="N193" s="25"/>
     </row>
     <row r="194" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="228"/>
-      <c r="B194" s="241"/>
+      <c r="A194" s="217"/>
+      <c r="B194" s="235"/>
       <c r="C194" s="154" t="s">
         <v>262</v>
       </c>
@@ -7807,8 +7807,8 @@
       <c r="N194" s="25"/>
     </row>
     <row r="195" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="228"/>
-      <c r="B195" s="242"/>
+      <c r="A195" s="217"/>
+      <c r="B195" s="233"/>
       <c r="C195" s="155" t="s">
         <v>106</v>
       </c>
@@ -7825,8 +7825,8 @@
       <c r="N195" s="26"/>
     </row>
     <row r="196" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="228"/>
-      <c r="B196" s="223" t="s">
+      <c r="A196" s="217"/>
+      <c r="B196" s="212" t="s">
         <v>263</v>
       </c>
       <c r="C196" s="13" t="s">
@@ -7845,8 +7845,8 @@
       <c r="N196" s="8"/>
     </row>
     <row r="197" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="228"/>
-      <c r="B197" s="221"/>
+      <c r="A197" s="217"/>
+      <c r="B197" s="213"/>
       <c r="C197" s="153" t="s">
         <v>264</v>
       </c>
@@ -7863,8 +7863,8 @@
       <c r="N197" s="25"/>
     </row>
     <row r="198" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="228"/>
-      <c r="B198" s="221"/>
+      <c r="A198" s="217"/>
+      <c r="B198" s="213"/>
       <c r="C198" s="154" t="s">
         <v>265</v>
       </c>
@@ -7881,8 +7881,8 @@
       <c r="N198" s="25"/>
     </row>
     <row r="199" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="228"/>
-      <c r="B199" s="221"/>
+      <c r="A199" s="217"/>
+      <c r="B199" s="213"/>
       <c r="C199" s="154" t="s">
         <v>266</v>
       </c>
@@ -7899,8 +7899,8 @@
       <c r="N199" s="25"/>
     </row>
     <row r="200" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="228"/>
-      <c r="B200" s="221"/>
+      <c r="A200" s="217"/>
+      <c r="B200" s="213"/>
       <c r="C200" s="154" t="s">
         <v>267</v>
       </c>
@@ -7917,8 +7917,8 @@
       <c r="N200" s="25"/>
     </row>
     <row r="201" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="228"/>
-      <c r="B201" s="221"/>
+      <c r="A201" s="217"/>
+      <c r="B201" s="213"/>
       <c r="C201" s="154" t="s">
         <v>106</v>
       </c>
@@ -7935,8 +7935,8 @@
       <c r="N201" s="25"/>
     </row>
     <row r="202" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="228"/>
-      <c r="B202" s="221"/>
+      <c r="A202" s="217"/>
+      <c r="B202" s="213"/>
       <c r="C202" s="13" t="s">
         <v>85</v>
       </c>
@@ -7953,8 +7953,8 @@
       <c r="N202" s="8"/>
     </row>
     <row r="203" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="228"/>
-      <c r="B203" s="221"/>
+      <c r="A203" s="217"/>
+      <c r="B203" s="213"/>
       <c r="C203" s="153" t="s">
         <v>268</v>
       </c>
@@ -7971,8 +7971,8 @@
       <c r="N203" s="25"/>
     </row>
     <row r="204" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="228"/>
-      <c r="B204" s="224"/>
+      <c r="A204" s="217"/>
+      <c r="B204" s="214"/>
       <c r="C204" s="155" t="s">
         <v>106</v>
       </c>
@@ -7989,8 +7989,8 @@
       <c r="N204" s="26"/>
     </row>
     <row r="205" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="228"/>
-      <c r="B205" s="223" t="s">
+      <c r="A205" s="217"/>
+      <c r="B205" s="212" t="s">
         <v>269</v>
       </c>
       <c r="C205" s="13" t="s">
@@ -8009,8 +8009,8 @@
       <c r="N205" s="8"/>
     </row>
     <row r="206" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="228"/>
-      <c r="B206" s="221"/>
+      <c r="A206" s="217"/>
+      <c r="B206" s="213"/>
       <c r="C206" s="153" t="s">
         <v>270</v>
       </c>
@@ -8027,8 +8027,8 @@
       <c r="N206" s="25"/>
     </row>
     <row r="207" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="228"/>
-      <c r="B207" s="221"/>
+      <c r="A207" s="217"/>
+      <c r="B207" s="213"/>
       <c r="C207" s="154" t="s">
         <v>271</v>
       </c>
@@ -8045,8 +8045,8 @@
       <c r="N207" s="25"/>
     </row>
     <row r="208" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="228"/>
-      <c r="B208" s="221"/>
+      <c r="A208" s="217"/>
+      <c r="B208" s="213"/>
       <c r="C208" s="154" t="s">
         <v>272</v>
       </c>
@@ -8063,8 +8063,8 @@
       <c r="N208" s="25"/>
     </row>
     <row r="209" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="228"/>
-      <c r="B209" s="221"/>
+      <c r="A209" s="217"/>
+      <c r="B209" s="213"/>
       <c r="C209" s="154" t="s">
         <v>106</v>
       </c>
@@ -8081,8 +8081,8 @@
       <c r="N209" s="25"/>
     </row>
     <row r="210" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="228"/>
-      <c r="B210" s="221"/>
+      <c r="A210" s="217"/>
+      <c r="B210" s="213"/>
       <c r="C210" s="13" t="s">
         <v>85</v>
       </c>
@@ -8099,8 +8099,8 @@
       <c r="N210" s="8"/>
     </row>
     <row r="211" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="228"/>
-      <c r="B211" s="221"/>
+      <c r="A211" s="217"/>
+      <c r="B211" s="213"/>
       <c r="C211" s="153" t="s">
         <v>273</v>
       </c>
@@ -8117,8 +8117,8 @@
       <c r="N211" s="25"/>
     </row>
     <row r="212" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="228"/>
-      <c r="B212" s="224"/>
+      <c r="A212" s="217"/>
+      <c r="B212" s="214"/>
       <c r="C212" s="155" t="s">
         <v>106</v>
       </c>
@@ -8135,8 +8135,8 @@
       <c r="N212" s="26"/>
     </row>
     <row r="213" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="228"/>
-      <c r="B213" s="223" t="s">
+      <c r="A213" s="217"/>
+      <c r="B213" s="212" t="s">
         <v>274</v>
       </c>
       <c r="C213" s="13" t="s">
@@ -8155,8 +8155,8 @@
       <c r="N213" s="8"/>
     </row>
     <row r="214" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="228"/>
-      <c r="B214" s="221"/>
+      <c r="A214" s="217"/>
+      <c r="B214" s="213"/>
       <c r="C214" s="153" t="s">
         <v>275</v>
       </c>
@@ -8173,8 +8173,8 @@
       <c r="N214" s="25"/>
     </row>
     <row r="215" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="228"/>
-      <c r="B215" s="221"/>
+      <c r="A215" s="217"/>
+      <c r="B215" s="213"/>
       <c r="C215" s="153" t="s">
         <v>276</v>
       </c>
@@ -8191,8 +8191,8 @@
       <c r="N215" s="25"/>
     </row>
     <row r="216" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="228"/>
-      <c r="B216" s="221"/>
+      <c r="A216" s="217"/>
+      <c r="B216" s="213"/>
       <c r="C216" s="154" t="s">
         <v>106</v>
       </c>
@@ -8209,8 +8209,8 @@
       <c r="N216" s="25"/>
     </row>
     <row r="217" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="228"/>
-      <c r="B217" s="221"/>
+      <c r="A217" s="217"/>
+      <c r="B217" s="213"/>
       <c r="C217" s="13" t="s">
         <v>85</v>
       </c>
@@ -8227,8 +8227,8 @@
       <c r="N217" s="8"/>
     </row>
     <row r="218" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="228"/>
-      <c r="B218" s="221"/>
+      <c r="A218" s="217"/>
+      <c r="B218" s="213"/>
       <c r="C218" s="153" t="s">
         <v>277</v>
       </c>
@@ -8245,8 +8245,8 @@
       <c r="N218" s="25"/>
     </row>
     <row r="219" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="228"/>
-      <c r="B219" s="221"/>
+      <c r="A219" s="217"/>
+      <c r="B219" s="213"/>
       <c r="C219" s="34" t="s">
         <v>278</v>
       </c>
@@ -8263,8 +8263,8 @@
       <c r="N219" s="28"/>
     </row>
     <row r="220" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="228"/>
-      <c r="B220" s="224"/>
+      <c r="A220" s="217"/>
+      <c r="B220" s="214"/>
       <c r="C220" s="155" t="s">
         <v>106</v>
       </c>
@@ -8281,8 +8281,8 @@
       <c r="N220" s="26"/>
     </row>
     <row r="221" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="228"/>
-      <c r="B221" s="223" t="s">
+      <c r="A221" s="217"/>
+      <c r="B221" s="212" t="s">
         <v>279</v>
       </c>
       <c r="C221" s="13" t="s">
@@ -8301,8 +8301,8 @@
       <c r="N221" s="8"/>
     </row>
     <row r="222" spans="1:14" s="189" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="228"/>
-      <c r="B222" s="221"/>
+      <c r="A222" s="217"/>
+      <c r="B222" s="213"/>
       <c r="C222" s="153" t="s">
         <v>280</v>
       </c>
@@ -8319,8 +8319,8 @@
       <c r="N222" s="24"/>
     </row>
     <row r="223" spans="1:14" s="189" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="228"/>
-      <c r="B223" s="221"/>
+      <c r="A223" s="217"/>
+      <c r="B223" s="213"/>
       <c r="C223" s="153" t="s">
         <v>281</v>
       </c>
@@ -8337,8 +8337,8 @@
       <c r="N223" s="24"/>
     </row>
     <row r="224" spans="1:14" s="189" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="228"/>
-      <c r="B224" s="221"/>
+      <c r="A224" s="217"/>
+      <c r="B224" s="213"/>
       <c r="C224" s="154" t="s">
         <v>106</v>
       </c>
@@ -8355,8 +8355,8 @@
       <c r="N224" s="25"/>
     </row>
     <row r="225" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="228"/>
-      <c r="B225" s="221"/>
+      <c r="A225" s="217"/>
+      <c r="B225" s="213"/>
       <c r="C225" s="13" t="s">
         <v>85</v>
       </c>
@@ -8373,8 +8373,8 @@
       <c r="N225" s="8"/>
     </row>
     <row r="226" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="228"/>
-      <c r="B226" s="221"/>
+      <c r="A226" s="217"/>
+      <c r="B226" s="213"/>
       <c r="C226" s="153" t="s">
         <v>282</v>
       </c>
@@ -8391,8 +8391,8 @@
       <c r="N226" s="25"/>
     </row>
     <row r="227" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="228"/>
-      <c r="B227" s="221"/>
+      <c r="A227" s="217"/>
+      <c r="B227" s="213"/>
       <c r="C227" s="34" t="s">
         <v>283</v>
       </c>
@@ -8409,8 +8409,8 @@
       <c r="N227" s="28"/>
     </row>
     <row r="228" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="228"/>
-      <c r="B228" s="224"/>
+      <c r="A228" s="217"/>
+      <c r="B228" s="214"/>
       <c r="C228" s="156" t="s">
         <v>106</v>
       </c>
@@ -8427,11 +8427,11 @@
       <c r="N228" s="28"/>
     </row>
     <row r="229" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="228"/>
-      <c r="B229" s="243" t="s">
+      <c r="A229" s="217"/>
+      <c r="B229" s="224" t="s">
         <v>284</v>
       </c>
-      <c r="C229" s="243"/>
+      <c r="C229" s="224"/>
       <c r="D229" s="76"/>
       <c r="E229" s="61"/>
       <c r="F229" s="61"/>
@@ -8445,8 +8445,8 @@
       <c r="N229" s="62"/>
     </row>
     <row r="230" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="228"/>
-      <c r="B230" s="223" t="s">
+      <c r="A230" s="217"/>
+      <c r="B230" s="212" t="s">
         <v>285</v>
       </c>
       <c r="C230" s="43" t="s">
@@ -8465,8 +8465,8 @@
       <c r="N230" s="8"/>
     </row>
     <row r="231" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="228"/>
-      <c r="B231" s="221"/>
+      <c r="A231" s="217"/>
+      <c r="B231" s="213"/>
       <c r="C231" s="154" t="s">
         <v>286</v>
       </c>
@@ -8483,8 +8483,8 @@
       <c r="N231" s="25"/>
     </row>
     <row r="232" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="228"/>
-      <c r="B232" s="221"/>
+      <c r="A232" s="217"/>
+      <c r="B232" s="213"/>
       <c r="C232" s="154" t="s">
         <v>287</v>
       </c>
@@ -8501,7 +8501,7 @@
       <c r="N232" s="25"/>
     </row>
     <row r="233" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="228"/>
+      <c r="A233" s="217"/>
       <c r="B233" s="33" t="s">
         <v>111</v>
       </c>
@@ -8521,8 +8521,8 @@
       <c r="N233" s="25"/>
     </row>
     <row r="234" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="228"/>
-      <c r="B234" s="212" t="s">
+      <c r="A234" s="217"/>
+      <c r="B234" s="221" t="s">
         <v>230</v>
       </c>
       <c r="C234" s="154" t="s">
@@ -8541,8 +8541,8 @@
       <c r="N234" s="25"/>
     </row>
     <row r="235" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="228"/>
-      <c r="B235" s="212"/>
+      <c r="A235" s="217"/>
+      <c r="B235" s="221"/>
       <c r="C235" s="154" t="s">
         <v>290</v>
       </c>
@@ -8559,8 +8559,8 @@
       <c r="N235" s="25"/>
     </row>
     <row r="236" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="228"/>
-      <c r="B236" s="212"/>
+      <c r="A236" s="217"/>
+      <c r="B236" s="221"/>
       <c r="C236" s="154" t="s">
         <v>291</v>
       </c>
@@ -8577,8 +8577,8 @@
       <c r="N236" s="25"/>
     </row>
     <row r="237" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="228"/>
-      <c r="B237" s="239"/>
+      <c r="A237" s="217"/>
+      <c r="B237" s="238"/>
       <c r="C237" s="154" t="s">
         <v>292</v>
       </c>
@@ -8595,8 +8595,8 @@
       <c r="N237" s="25"/>
     </row>
     <row r="238" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="228"/>
-      <c r="B238" s="239"/>
+      <c r="A238" s="217"/>
+      <c r="B238" s="238"/>
       <c r="C238" s="154" t="s">
         <v>293</v>
       </c>
@@ -8613,7 +8613,7 @@
       <c r="N238" s="25"/>
     </row>
     <row r="239" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="228"/>
+      <c r="A239" s="217"/>
       <c r="C239" s="154" t="s">
         <v>106</v>
       </c>
@@ -8630,7 +8630,7 @@
       <c r="N239" s="25"/>
     </row>
     <row r="240" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="228"/>
+      <c r="A240" s="217"/>
       <c r="C240" s="13" t="s">
         <v>85</v>
       </c>
@@ -8647,7 +8647,7 @@
       <c r="N240" s="8"/>
     </row>
     <row r="241" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="228"/>
+      <c r="A241" s="217"/>
       <c r="C241" s="153" t="s">
         <v>294</v>
       </c>
@@ -8664,7 +8664,7 @@
       <c r="N241" s="25"/>
     </row>
     <row r="242" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="228"/>
+      <c r="A242" s="217"/>
       <c r="C242" s="154" t="s">
         <v>295</v>
       </c>
@@ -8681,7 +8681,7 @@
       <c r="N242" s="25"/>
     </row>
     <row r="243" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="228"/>
+      <c r="A243" s="217"/>
       <c r="C243" s="154" t="s">
         <v>296</v>
       </c>
@@ -8698,7 +8698,7 @@
       <c r="N243" s="25"/>
     </row>
     <row r="244" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="229"/>
+      <c r="A244" s="218"/>
       <c r="B244" s="7"/>
       <c r="C244" s="155" t="s">
         <v>106</v>
@@ -8716,11 +8716,11 @@
       <c r="N244" s="26"/>
     </row>
     <row r="245" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="238" t="s">
+      <c r="A245" s="237" t="s">
         <v>297</v>
       </c>
-      <c r="B245" s="238"/>
-      <c r="C245" s="238"/>
+      <c r="B245" s="237"/>
+      <c r="C245" s="237"/>
       <c r="D245" s="77"/>
       <c r="E245" s="17"/>
       <c r="F245" s="17"/>
@@ -8734,11 +8734,11 @@
       <c r="N245" s="41"/>
     </row>
     <row r="246" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="237" t="s">
+      <c r="A246" s="239" t="s">
         <v>298</v>
       </c>
-      <c r="B246" s="237"/>
-      <c r="C246" s="237"/>
+      <c r="B246" s="239"/>
+      <c r="C246" s="239"/>
       <c r="D246" s="70"/>
       <c r="E246" s="42"/>
       <c r="F246" s="42"/>
@@ -8752,10 +8752,10 @@
       <c r="N246" s="45"/>
     </row>
     <row r="247" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="228" t="s">
+      <c r="A247" s="217" t="s">
         <v>299</v>
       </c>
-      <c r="B247" s="221" t="s">
+      <c r="B247" s="213" t="s">
         <v>300</v>
       </c>
       <c r="C247" s="43" t="s">
@@ -8774,8 +8774,8 @@
       <c r="N247" s="44"/>
     </row>
     <row r="248" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="228"/>
-      <c r="B248" s="221"/>
+      <c r="A248" s="217"/>
+      <c r="B248" s="213"/>
       <c r="C248" s="154" t="s">
         <v>301</v>
       </c>
@@ -8792,8 +8792,8 @@
       <c r="N248" s="25"/>
     </row>
     <row r="249" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="228"/>
-      <c r="B249" s="221"/>
+      <c r="A249" s="217"/>
+      <c r="B249" s="213"/>
       <c r="C249" s="154" t="s">
         <v>302</v>
       </c>
@@ -8810,8 +8810,8 @@
       <c r="N249" s="25"/>
     </row>
     <row r="250" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="228"/>
-      <c r="B250" s="221"/>
+      <c r="A250" s="217"/>
+      <c r="B250" s="213"/>
       <c r="C250" s="154" t="s">
         <v>303</v>
       </c>
@@ -8828,7 +8828,7 @@
       <c r="N250" s="25"/>
     </row>
     <row r="251" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="228"/>
+      <c r="A251" s="217"/>
       <c r="B251" s="33" t="s">
         <v>111</v>
       </c>
@@ -8848,8 +8848,8 @@
       <c r="N251" s="25"/>
     </row>
     <row r="252" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="228"/>
-      <c r="B252" s="212" t="s">
+      <c r="A252" s="217"/>
+      <c r="B252" s="221" t="s">
         <v>304</v>
       </c>
       <c r="C252" s="13" t="s">
@@ -8868,8 +8868,8 @@
       <c r="N252" s="8"/>
     </row>
     <row r="253" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="228"/>
-      <c r="B253" s="212"/>
+      <c r="A253" s="217"/>
+      <c r="B253" s="221"/>
       <c r="C253" s="153" t="s">
         <v>305</v>
       </c>
@@ -8886,8 +8886,8 @@
       <c r="N253" s="25"/>
     </row>
     <row r="254" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="229"/>
-      <c r="B254" s="213"/>
+      <c r="A254" s="218"/>
+      <c r="B254" s="236"/>
       <c r="C254" s="155" t="s">
         <v>106</v>
       </c>
@@ -8904,11 +8904,11 @@
       <c r="N254" s="26"/>
     </row>
     <row r="255" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="230" t="s">
+      <c r="A255" s="223" t="s">
         <v>306</v>
       </c>
-      <c r="B255" s="230"/>
-      <c r="C255" s="230"/>
+      <c r="B255" s="223"/>
+      <c r="C255" s="223"/>
       <c r="D255" s="70"/>
       <c r="E255" s="42"/>
       <c r="F255" s="42"/>
@@ -8922,10 +8922,10 @@
       <c r="N255" s="45"/>
     </row>
     <row r="256" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A256" s="228" t="s">
+      <c r="A256" s="217" t="s">
         <v>307</v>
       </c>
-      <c r="B256" s="221" t="s">
+      <c r="B256" s="213" t="s">
         <v>308</v>
       </c>
       <c r="C256" s="43" t="s">
@@ -8944,8 +8944,8 @@
       <c r="N256" s="44"/>
     </row>
     <row r="257" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="228"/>
-      <c r="B257" s="221"/>
+      <c r="A257" s="217"/>
+      <c r="B257" s="213"/>
       <c r="C257" s="154" t="s">
         <v>309</v>
       </c>
@@ -8962,8 +8962,8 @@
       <c r="N257" s="25"/>
     </row>
     <row r="258" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="228"/>
-      <c r="B258" s="221"/>
+      <c r="A258" s="217"/>
+      <c r="B258" s="213"/>
       <c r="C258" s="154" t="s">
         <v>310</v>
       </c>
@@ -8980,8 +8980,8 @@
       <c r="N258" s="25"/>
     </row>
     <row r="259" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="228"/>
-      <c r="B259" s="221"/>
+      <c r="A259" s="217"/>
+      <c r="B259" s="213"/>
       <c r="C259" s="154" t="s">
         <v>311</v>
       </c>
@@ -8998,8 +8998,8 @@
       <c r="N259" s="25"/>
     </row>
     <row r="260" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="228"/>
-      <c r="B260" s="221"/>
+      <c r="A260" s="217"/>
+      <c r="B260" s="213"/>
       <c r="C260" s="154" t="s">
         <v>106</v>
       </c>
@@ -9016,8 +9016,8 @@
       <c r="N260" s="25"/>
     </row>
     <row r="261" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="228"/>
-      <c r="B261" s="221"/>
+      <c r="A261" s="217"/>
+      <c r="B261" s="213"/>
       <c r="C261" s="13" t="s">
         <v>85</v>
       </c>
@@ -9034,8 +9034,8 @@
       <c r="N261" s="8"/>
     </row>
     <row r="262" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="228"/>
-      <c r="B262" s="221"/>
+      <c r="A262" s="217"/>
+      <c r="B262" s="213"/>
       <c r="C262" s="153" t="s">
         <v>312</v>
       </c>
@@ -9052,8 +9052,8 @@
       <c r="N262" s="25"/>
     </row>
     <row r="263" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A263" s="228"/>
-      <c r="B263" s="221"/>
+      <c r="A263" s="217"/>
+      <c r="B263" s="213"/>
       <c r="C263" s="154" t="s">
         <v>313</v>
       </c>
@@ -9070,8 +9070,8 @@
       <c r="N263" s="25"/>
     </row>
     <row r="264" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A264" s="228"/>
-      <c r="B264" s="224"/>
+      <c r="A264" s="217"/>
+      <c r="B264" s="214"/>
       <c r="C264" s="155" t="s">
         <v>106</v>
       </c>
@@ -9088,7 +9088,7 @@
       <c r="N264" s="26"/>
     </row>
     <row r="265" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="228"/>
+      <c r="A265" s="217"/>
       <c r="B265" s="240" t="s">
         <v>314</v>
       </c>
@@ -9108,8 +9108,8 @@
       <c r="N265" s="8"/>
     </row>
     <row r="266" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="228"/>
-      <c r="B266" s="241"/>
+      <c r="A266" s="217"/>
+      <c r="B266" s="235"/>
       <c r="C266" s="153" t="s">
         <v>315</v>
       </c>
@@ -9126,8 +9126,8 @@
       <c r="N266" s="24"/>
     </row>
     <row r="267" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="228"/>
-      <c r="B267" s="241"/>
+      <c r="A267" s="217"/>
+      <c r="B267" s="235"/>
       <c r="C267" s="154" t="s">
         <v>106</v>
       </c>
@@ -9144,8 +9144,8 @@
       <c r="N267" s="25"/>
     </row>
     <row r="268" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A268" s="228"/>
-      <c r="B268" s="241"/>
+      <c r="A268" s="217"/>
+      <c r="B268" s="235"/>
       <c r="C268" s="13" t="s">
         <v>85</v>
       </c>
@@ -9162,8 +9162,8 @@
       <c r="N268" s="8"/>
     </row>
     <row r="269" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="228"/>
-      <c r="B269" s="241"/>
+      <c r="A269" s="217"/>
+      <c r="B269" s="235"/>
       <c r="C269" s="153" t="s">
         <v>316</v>
       </c>
@@ -9180,8 +9180,8 @@
       <c r="N269" s="25"/>
     </row>
     <row r="270" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="229"/>
-      <c r="B270" s="242"/>
+      <c r="A270" s="218"/>
+      <c r="B270" s="233"/>
       <c r="C270" s="155" t="s">
         <v>106</v>
       </c>
@@ -9198,11 +9198,11 @@
       <c r="N270" s="26"/>
     </row>
     <row r="271" spans="1:14" s="184" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A271" s="230" t="s">
+      <c r="A271" s="223" t="s">
         <v>205</v>
       </c>
-      <c r="B271" s="230"/>
-      <c r="C271" s="230"/>
+      <c r="B271" s="223"/>
+      <c r="C271" s="223"/>
       <c r="D271" s="70"/>
       <c r="E271" s="42"/>
       <c r="F271" s="42"/>
@@ -9216,10 +9216,10 @@
       <c r="N271" s="45"/>
     </row>
     <row r="272" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A272" s="228" t="s">
+      <c r="A272" s="217" t="s">
         <v>317</v>
       </c>
-      <c r="B272" s="221" t="s">
+      <c r="B272" s="213" t="s">
         <v>318</v>
       </c>
       <c r="C272" s="43" t="s">
@@ -9238,8 +9238,8 @@
       <c r="N272" s="44"/>
     </row>
     <row r="273" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A273" s="228"/>
-      <c r="B273" s="221"/>
+      <c r="A273" s="217"/>
+      <c r="B273" s="213"/>
       <c r="C273" s="154" t="s">
         <v>319</v>
       </c>
@@ -9256,8 +9256,8 @@
       <c r="N273" s="25"/>
     </row>
     <row r="274" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="228"/>
-      <c r="B274" s="221"/>
+      <c r="A274" s="217"/>
+      <c r="B274" s="213"/>
       <c r="C274" s="154" t="s">
         <v>320</v>
       </c>
@@ -9274,8 +9274,8 @@
       <c r="N274" s="25"/>
     </row>
     <row r="275" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A275" s="228"/>
-      <c r="B275" s="221"/>
+      <c r="A275" s="217"/>
+      <c r="B275" s="213"/>
       <c r="C275" s="154" t="s">
         <v>321</v>
       </c>
@@ -9292,8 +9292,8 @@
       <c r="N275" s="25"/>
     </row>
     <row r="276" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="228"/>
-      <c r="B276" s="221"/>
+      <c r="A276" s="217"/>
+      <c r="B276" s="213"/>
       <c r="C276" s="154" t="s">
         <v>322</v>
       </c>
@@ -9310,8 +9310,8 @@
       <c r="N276" s="25"/>
     </row>
     <row r="277" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A277" s="228"/>
-      <c r="B277" s="221"/>
+      <c r="A277" s="217"/>
+      <c r="B277" s="213"/>
       <c r="C277" s="154" t="s">
         <v>106</v>
       </c>
@@ -9328,8 +9328,8 @@
       <c r="N277" s="25"/>
     </row>
     <row r="278" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A278" s="228"/>
-      <c r="B278" s="221"/>
+      <c r="A278" s="217"/>
+      <c r="B278" s="213"/>
       <c r="C278" s="13" t="s">
         <v>85</v>
       </c>
@@ -9346,8 +9346,8 @@
       <c r="N278" s="8"/>
     </row>
     <row r="279" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A279" s="228"/>
-      <c r="B279" s="221"/>
+      <c r="A279" s="217"/>
+      <c r="B279" s="213"/>
       <c r="C279" s="153" t="s">
         <v>323</v>
       </c>
@@ -9364,8 +9364,8 @@
       <c r="N279" s="25"/>
     </row>
     <row r="280" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A280" s="228"/>
-      <c r="B280" s="221"/>
+      <c r="A280" s="217"/>
+      <c r="B280" s="213"/>
       <c r="C280" s="154" t="s">
         <v>324</v>
       </c>
@@ -9382,8 +9382,8 @@
       <c r="N280" s="25"/>
     </row>
     <row r="281" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A281" s="228"/>
-      <c r="B281" s="221"/>
+      <c r="A281" s="217"/>
+      <c r="B281" s="213"/>
       <c r="C281" s="154" t="s">
         <v>325</v>
       </c>
@@ -9400,8 +9400,8 @@
       <c r="N281" s="25"/>
     </row>
     <row r="282" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A282" s="228"/>
-      <c r="B282" s="224"/>
+      <c r="A282" s="217"/>
+      <c r="B282" s="214"/>
       <c r="C282" s="155" t="s">
         <v>106</v>
       </c>
@@ -9418,8 +9418,8 @@
       <c r="N282" s="26"/>
     </row>
     <row r="283" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A283" s="228"/>
-      <c r="B283" s="223" t="s">
+      <c r="A283" s="217"/>
+      <c r="B283" s="212" t="s">
         <v>326</v>
       </c>
       <c r="C283" s="13" t="s">
@@ -9438,8 +9438,8 @@
       <c r="N283" s="8"/>
     </row>
     <row r="284" spans="1:14" s="189" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A284" s="228"/>
-      <c r="B284" s="221"/>
+      <c r="A284" s="217"/>
+      <c r="B284" s="213"/>
       <c r="C284" s="154" t="s">
         <v>327</v>
       </c>
@@ -9456,8 +9456,8 @@
       <c r="N284" s="25"/>
     </row>
     <row r="285" spans="1:14" s="189" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="228"/>
-      <c r="B285" s="221"/>
+      <c r="A285" s="217"/>
+      <c r="B285" s="213"/>
       <c r="C285" s="154" t="s">
         <v>106</v>
       </c>
@@ -9474,8 +9474,8 @@
       <c r="N285" s="25"/>
     </row>
     <row r="286" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="228"/>
-      <c r="B286" s="221"/>
+      <c r="A286" s="217"/>
+      <c r="B286" s="213"/>
       <c r="C286" s="13" t="s">
         <v>85</v>
       </c>
@@ -9492,8 +9492,8 @@
       <c r="N286" s="8"/>
     </row>
     <row r="287" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="228"/>
-      <c r="B287" s="221"/>
+      <c r="A287" s="217"/>
+      <c r="B287" s="213"/>
       <c r="C287" s="153" t="s">
         <v>328</v>
       </c>
@@ -9510,8 +9510,8 @@
       <c r="N287" s="25"/>
     </row>
     <row r="288" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A288" s="229"/>
-      <c r="B288" s="224"/>
+      <c r="A288" s="218"/>
+      <c r="B288" s="214"/>
       <c r="C288" s="155" t="s">
         <v>106</v>
       </c>
@@ -9529,6 +9529,78 @@
     </row>
   </sheetData>
   <mergeCells count="88">
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B24:B31"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B247:B250"/>
+    <mergeCell ref="B252:B254"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="B75:B80"/>
+    <mergeCell ref="D53:N53"/>
+    <mergeCell ref="A66:A88"/>
+    <mergeCell ref="A51:A63"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="J1:K2"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="L1:M2"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A185:C185"/>
+    <mergeCell ref="B283:B288"/>
+    <mergeCell ref="B256:B264"/>
+    <mergeCell ref="B205:B212"/>
+    <mergeCell ref="A245:C245"/>
+    <mergeCell ref="A271:C271"/>
+    <mergeCell ref="B237:B238"/>
+    <mergeCell ref="A246:C246"/>
+    <mergeCell ref="A272:A288"/>
+    <mergeCell ref="B230:B232"/>
+    <mergeCell ref="A256:A270"/>
+    <mergeCell ref="A247:A254"/>
+    <mergeCell ref="B234:B236"/>
+    <mergeCell ref="B272:B282"/>
+    <mergeCell ref="B265:B270"/>
+    <mergeCell ref="A90:A101"/>
+    <mergeCell ref="B145:B147"/>
+    <mergeCell ref="B213:B220"/>
+    <mergeCell ref="A255:C255"/>
+    <mergeCell ref="B42:B49"/>
+    <mergeCell ref="A141:C141"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="B196:B204"/>
+    <mergeCell ref="B174:B184"/>
+    <mergeCell ref="B221:B228"/>
+    <mergeCell ref="B186:B195"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="B166:B173"/>
+    <mergeCell ref="B153:B154"/>
+    <mergeCell ref="B156:B161"/>
+    <mergeCell ref="A103:A119"/>
+    <mergeCell ref="B81:B88"/>
+    <mergeCell ref="A102:C102"/>
+    <mergeCell ref="A186:A244"/>
+    <mergeCell ref="B229:C229"/>
+    <mergeCell ref="F8:M8"/>
+    <mergeCell ref="A8:A16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:A40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A120:C120"/>
+    <mergeCell ref="A89:C89"/>
     <mergeCell ref="B32:B40"/>
     <mergeCell ref="B60:B61"/>
     <mergeCell ref="B51:B53"/>
@@ -9545,78 +9617,6 @@
     <mergeCell ref="B90:B101"/>
     <mergeCell ref="B114:B119"/>
     <mergeCell ref="B103:B113"/>
-    <mergeCell ref="B81:B88"/>
-    <mergeCell ref="A102:C102"/>
-    <mergeCell ref="A186:A244"/>
-    <mergeCell ref="B229:C229"/>
-    <mergeCell ref="F8:M8"/>
-    <mergeCell ref="A8:A16"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:A40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A120:C120"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A90:A101"/>
-    <mergeCell ref="B145:B147"/>
-    <mergeCell ref="B213:B220"/>
-    <mergeCell ref="A255:C255"/>
-    <mergeCell ref="B42:B49"/>
-    <mergeCell ref="A141:C141"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="B196:B204"/>
-    <mergeCell ref="B174:B184"/>
-    <mergeCell ref="B221:B228"/>
-    <mergeCell ref="B186:B195"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="B166:B173"/>
-    <mergeCell ref="B153:B154"/>
-    <mergeCell ref="B156:B161"/>
-    <mergeCell ref="A103:A119"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A185:C185"/>
-    <mergeCell ref="B283:B288"/>
-    <mergeCell ref="B256:B264"/>
-    <mergeCell ref="B205:B212"/>
-    <mergeCell ref="A245:C245"/>
-    <mergeCell ref="A271:C271"/>
-    <mergeCell ref="B237:B238"/>
-    <mergeCell ref="A246:C246"/>
-    <mergeCell ref="A272:A288"/>
-    <mergeCell ref="B230:B232"/>
-    <mergeCell ref="A256:A270"/>
-    <mergeCell ref="A247:A254"/>
-    <mergeCell ref="B234:B236"/>
-    <mergeCell ref="B272:B282"/>
-    <mergeCell ref="B265:B270"/>
-    <mergeCell ref="B247:B250"/>
-    <mergeCell ref="B252:B254"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="B75:B80"/>
-    <mergeCell ref="D53:N53"/>
-    <mergeCell ref="A66:A88"/>
-    <mergeCell ref="A51:A63"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="J1:K2"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="L1:M2"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:B31"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="K1:M1048576">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>